<commit_message>
Additional data and comments for day
</commit_message>
<xml_diff>
--- a/polynomial-trendlines/all-day-glucose.xlsx
+++ b/polynomial-trendlines/all-day-glucose.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="224">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -860,11 +860,15 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">mostly 10x10; 7 PUs</t>
+      <t xml:space="preserve">mostly 10x10; 7 PUs
+Lots of non-keto pasta for dinner</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">2024-03-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:30 PM: Freestyle Libré. 6:40: 1 Voortman Choc Chip cookie (cars, 12 gm).</t>
   </si>
   <si>
     <t xml:space="preserve">2024-03-28</t>
@@ -1334,7 +1338,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart91.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart146.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2312,7 +2316,10 @@
                   <c:v>116.571428571429</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>118.857142857143</c:v>
+                  <c:v>118.2</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>115.142857142857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2327,11 +2334,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="9980697"/>
-        <c:axId val="91042384"/>
+        <c:axId val="42624221"/>
+        <c:axId val="31828434"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="9980697"/>
+        <c:axId val="42624221"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2359,7 +2366,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91042384"/>
+        <c:crossAx val="31828434"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2367,7 +2374,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91042384"/>
+        <c:axId val="31828434"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="155"/>
@@ -2442,7 +2449,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9980697"/>
+        <c:crossAx val="42624221"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -2504,7 +2511,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart92.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart147.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3448,6 +3455,9 @@
                 <c:pt idx="131">
                   <c:v>105</c:v>
                 </c:pt>
+                <c:pt idx="132">
+                  <c:v>109</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3461,11 +3471,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="63707665"/>
-        <c:axId val="46260314"/>
+        <c:axId val="14127650"/>
+        <c:axId val="49404034"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63707665"/>
+        <c:axId val="14127650"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3493,7 +3503,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46260314"/>
+        <c:crossAx val="49404034"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3501,7 +3511,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46260314"/>
+        <c:axId val="49404034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -3540,7 +3550,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="63707665"/>
+        <c:crossAx val="14127650"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -3602,7 +3612,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart93.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart148.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3764,16 +3774,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>116.625</c:v>
+                  <c:v>116.557522123894</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129.533333333333</c:v>
+                  <c:v>130.064516129032</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>136.163265306122</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>126.142857142857</c:v>
+                  <c:v>125.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>127.392156862745</c:v>
@@ -3782,34 +3792,34 @@
                   <c:v>117.962962962963</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>133.714285714286</c:v>
+                  <c:v>133.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>125.782608695652</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130.372093023256</c:v>
+                  <c:v>130.181818181818</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>125.264150943396</c:v>
+                  <c:v>125.240740740741</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>124.196428571429</c:v>
+                  <c:v>123.684210526316</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>126.829787234043</c:v>
+                  <c:v>126.4375</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>121.893617021277</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>127.19512195122</c:v>
+                  <c:v>126.261904761905</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>135.125</c:v>
+                  <c:v>135.754385964912</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>123.5</c:v>
+                  <c:v>122.949152542373</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3817,11 +3827,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="42943639"/>
-        <c:axId val="70512595"/>
+        <c:axId val="31641833"/>
+        <c:axId val="24780442"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42943639"/>
+        <c:axId val="31641833"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3885,7 +3895,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70512595"/>
+        <c:crossAx val="24780442"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3893,7 +3903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70512595"/>
+        <c:axId val="24780442"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="110"/>
@@ -3959,7 +3969,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42943639"/>
+        <c:crossAx val="31641833"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4010,7 +4020,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart94.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart149.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4931,11 +4941,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="14565463"/>
-        <c:axId val="94103073"/>
+        <c:axId val="87840645"/>
+        <c:axId val="81503216"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="14565463"/>
+        <c:axId val="87840645"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45413"/>
@@ -4965,7 +4975,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94103073"/>
+        <c:crossAx val="81503216"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -4975,7 +4985,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="94103073"/>
+        <c:axId val="81503216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -5014,7 +5024,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14565463"/>
+        <c:crossAx val="87840645"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -5079,7 +5089,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart95.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart150.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7091,11 +7101,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="87765171"/>
-        <c:axId val="73228035"/>
+        <c:axId val="71033694"/>
+        <c:axId val="93884113"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87765171"/>
+        <c:axId val="71033694"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7123,7 +7133,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73228035"/>
+        <c:crossAx val="93884113"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7131,7 +7141,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73228035"/>
+        <c:axId val="93884113"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -7170,7 +7180,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87765171"/>
+        <c:crossAx val="71033694"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -7410,7 +7420,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4532" topLeftCell="C131" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="O134" activeCellId="0" sqref="O134"/>
+      <selection pane="bottomLeft" activeCell="U135" activeCellId="0" sqref="U135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12739,7 +12749,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
         <v>210</v>
       </c>
@@ -12748,7 +12758,7 @@
       </c>
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
-      <c r="E134" s="2" t="n">
+      <c r="E134" s="32" t="n">
         <v>144</v>
       </c>
       <c r="F134" s="2" t="n">
@@ -12762,7 +12772,7 @@
       </c>
       <c r="I134" s="2"/>
       <c r="J134" s="2"/>
-      <c r="K134" s="2" t="n">
+      <c r="K134" s="32" t="n">
         <v>161</v>
       </c>
       <c r="L134" s="2" t="n">
@@ -12772,43 +12782,72 @@
       <c r="N134" s="30" t="n">
         <v>98</v>
       </c>
-      <c r="P134" s="2"/>
-      <c r="Q134" s="2"/>
+      <c r="O134" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="P134" s="32" t="n">
+        <v>171</v>
+      </c>
+      <c r="Q134" s="2" t="n">
+        <v>91</v>
+      </c>
       <c r="R134" s="18" t="n">
         <f aca="false">AVERAGEIF($C134:$Q134,"&gt;0")</f>
-        <v>118.857142857143</v>
+        <v>118.2</v>
       </c>
       <c r="U134" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C135" s="2"/>
+      <c r="B135" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="C135" s="32" t="n">
+        <v>146</v>
+      </c>
       <c r="D135" s="2"/>
-      <c r="E135" s="2"/>
+      <c r="E135" s="2" t="n">
+        <v>102</v>
+      </c>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
-      <c r="H135" s="30" t="s">
-        <v>185</v>
+      <c r="H135" s="30" t="n">
+        <v>109</v>
       </c>
       <c r="I135" s="2"/>
-      <c r="J135" s="2"/>
-      <c r="K135" s="2"/>
-      <c r="L135" s="2"/>
-      <c r="M135" s="2"/>
+      <c r="J135" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="K135" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="L135" s="2" t="n">
+        <v>95</v>
+      </c>
+      <c r="M135" s="2" t="n">
+        <v>108</v>
+      </c>
       <c r="N135" s="2"/>
       <c r="O135" s="30" t="s">
         <v>185</v>
       </c>
       <c r="P135" s="2"/>
       <c r="Q135" s="2"/>
+      <c r="R135" s="18" t="n">
+        <f aca="false">AVERAGEIF($C135:$Q135,"&gt;0")</f>
+        <v>115.142857142857</v>
+      </c>
+      <c r="U135" s="5" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
@@ -12831,22 +12870,22 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -12900,24 +12939,24 @@
         <v>0</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="n">
         <f aca="true">TODAY()</f>
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!B$3:B$159, "&gt;0")</f>
-        <v>116.625</v>
+        <v>116.557522123894</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -12927,7 +12966,7 @@
       </c>
       <c r="C4" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!C$3:C$153, "&gt;0")</f>
-        <v>129.533333333333</v>
+        <v>130.064516129032</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -12947,7 +12986,7 @@
       </c>
       <c r="C6" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!E$3:E$153, "&gt;0")</f>
-        <v>126.142857142857</v>
+        <v>125.66</v>
       </c>
       <c r="D6" s="7"/>
     </row>
@@ -12977,7 +13016,7 @@
       </c>
       <c r="C9" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!H$3:H$153, "&gt;0")</f>
-        <v>133.714285714286</v>
+        <v>133.22</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -12997,7 +13036,7 @@
       </c>
       <c r="C11" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!J$3:J$153, "&gt;0")</f>
-        <v>130.372093023256</v>
+        <v>130.181818181818</v>
       </c>
       <c r="D11" s="7"/>
     </row>
@@ -13007,7 +13046,7 @@
       </c>
       <c r="C12" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!K$3:K$153, "&gt;0")</f>
-        <v>125.264150943396</v>
+        <v>125.240740740741</v>
       </c>
       <c r="D12" s="7"/>
     </row>
@@ -13017,7 +13056,7 @@
       </c>
       <c r="C13" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!L$3:L$153, "&gt;0")</f>
-        <v>124.196428571429</v>
+        <v>123.684210526316</v>
       </c>
       <c r="D13" s="7"/>
     </row>
@@ -13027,7 +13066,7 @@
       </c>
       <c r="C14" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!M$3:M$153, "&gt;0")</f>
-        <v>126.829787234043</v>
+        <v>126.4375</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -13047,7 +13086,7 @@
       </c>
       <c r="C16" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!O$3:O$153, "&gt;0")</f>
-        <v>127.19512195122</v>
+        <v>126.261904761905</v>
       </c>
       <c r="D16" s="7"/>
     </row>
@@ -13057,7 +13096,7 @@
       </c>
       <c r="C17" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!P$3:P$153, "&gt;0")</f>
-        <v>135.125</v>
+        <v>135.754385964912</v>
       </c>
       <c r="D17" s="7"/>
     </row>
@@ -13067,7 +13106,7 @@
       </c>
       <c r="C18" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!Q$3:Q$159, "&gt;0")</f>
-        <v>123.5</v>
+        <v>122.949152542373</v>
       </c>
       <c r="D18" s="7"/>
     </row>
@@ -13086,7 +13125,7 @@
         <v>10</v>
       </c>
       <c r="U95" s="7" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13104,7 +13143,7 @@
         <v>117</v>
       </c>
       <c r="U113" s="49" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13166,7 +13205,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E1" s="2" t="n">
         <v>0</v>
@@ -13213,7 +13252,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
@@ -13260,7 +13299,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -13307,7 +13346,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>0</v>
@@ -13354,7 +13393,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>0</v>
@@ -13401,7 +13440,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0</v>
@@ -13448,7 +13487,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Add data to regression notebook and glucose spreadsheet
</commit_message>
<xml_diff>
--- a/polynomial-trendlines/all-day-glucose.xlsx
+++ b/polynomial-trendlines/all-day-glucose.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="224">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -868,7 +868,11 @@
     <t xml:space="preserve">2024-03-27</t>
   </si>
   <si>
-    <t xml:space="preserve">6:30 PM: Freestyle Libré. 6:40: 1 Voortman Choc Chip cookie (cars, 12 gm).</t>
+    <t xml:space="preserve">6:30 PM: Freestyle Libré. 6:40: 1 Voortman Choc Chip cookie (carbs, 12 gm). Glu rose to 160; -&gt;
+6:45: treadmill, 15m, 2.8 mph, 6%, 127 Cal, HR 120. Glu increase reversed abrupty; level dropped to 104 at 7:30.
+9 PM: Dinner. glu up to 161 before Irish Cream @ 9:30. 9: 35: Peak: 166.
+9:45: Treadmill, 20m, 2.5 mph, 5.5%, 140 Cal. Glu peaked at 202 ≈5 min after end.
+11:45 AM: Two isometric pull-ups. 12:11 AM: glu 134</t>
   </si>
   <si>
     <t xml:space="preserve">2024-03-28</t>
@@ -1338,7 +1342,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart146.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart186.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2319,7 +2323,7 @@
                   <c:v>118.2</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>115.142857142857</c:v>
+                  <c:v>126.545454545455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2334,11 +2338,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="42624221"/>
-        <c:axId val="31828434"/>
+        <c:axId val="32662322"/>
+        <c:axId val="1573105"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42624221"/>
+        <c:axId val="32662322"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2366,7 +2370,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31828434"/>
+        <c:crossAx val="1573105"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2374,7 +2378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31828434"/>
+        <c:axId val="1573105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="155"/>
@@ -2449,7 +2453,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42624221"/>
+        <c:crossAx val="32662322"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -2511,7 +2515,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart147.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart187.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3458,6 +3462,9 @@
                 <c:pt idx="132">
                   <c:v>109</c:v>
                 </c:pt>
+                <c:pt idx="133">
+                  <c:v>119</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3471,11 +3478,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="14127650"/>
-        <c:axId val="49404034"/>
+        <c:axId val="87844347"/>
+        <c:axId val="56868977"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14127650"/>
+        <c:axId val="87844347"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3503,7 +3510,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49404034"/>
+        <c:crossAx val="56868977"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3511,7 +3518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49404034"/>
+        <c:axId val="56868977"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -3550,7 +3557,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14127650"/>
+        <c:crossAx val="87844347"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -3612,7 +3619,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart148.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart188.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3774,7 +3781,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>116.557522123894</c:v>
+                  <c:v>116.578947368421</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>130.064516129032</c:v>
@@ -3810,16 +3817,16 @@
                   <c:v>126.4375</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>121.893617021277</c:v>
+                  <c:v>122.0625</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>126.261904761905</c:v>
+                  <c:v>126.348837209302</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>135.754385964912</c:v>
+                  <c:v>135.568965517241</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>122.949152542373</c:v>
+                  <c:v>124.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3827,11 +3834,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="31641833"/>
-        <c:axId val="24780442"/>
+        <c:axId val="90558165"/>
+        <c:axId val="73345214"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="31641833"/>
+        <c:axId val="90558165"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3895,7 +3902,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24780442"/>
+        <c:crossAx val="73345214"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3903,7 +3910,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="24780442"/>
+        <c:axId val="73345214"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="110"/>
@@ -3969,7 +3976,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31641833"/>
+        <c:crossAx val="90558165"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4020,7 +4027,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart149.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart189.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4941,11 +4948,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="87840645"/>
-        <c:axId val="81503216"/>
+        <c:axId val="84820420"/>
+        <c:axId val="41054328"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="87840645"/>
+        <c:axId val="84820420"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45413"/>
@@ -4975,7 +4982,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81503216"/>
+        <c:crossAx val="41054328"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -4985,7 +4992,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="81503216"/>
+        <c:axId val="41054328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -5024,7 +5031,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87840645"/>
+        <c:crossAx val="84820420"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -5089,7 +5096,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart150.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart190.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7101,11 +7108,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="71033694"/>
-        <c:axId val="93884113"/>
+        <c:axId val="38087513"/>
+        <c:axId val="57775575"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71033694"/>
+        <c:axId val="38087513"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7133,7 +7140,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93884113"/>
+        <c:crossAx val="57775575"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7141,7 +7148,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93884113"/>
+        <c:axId val="57775575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -7180,7 +7187,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71033694"/>
+        <c:crossAx val="38087513"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -7418,9 +7425,9 @@
   <dimension ref="A1:AM140"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4532" topLeftCell="C131" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="4532" topLeftCell="C133" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="U135" activeCellId="0" sqref="U135"/>
+      <selection pane="bottomLeft" activeCell="C136" activeCellId="0" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12799,7 +12806,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="134.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>212</v>
       </c>
@@ -12831,15 +12838,21 @@
       <c r="M135" s="2" t="n">
         <v>108</v>
       </c>
-      <c r="N135" s="2"/>
-      <c r="O135" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="P135" s="2"/>
-      <c r="Q135" s="2"/>
+      <c r="N135" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="O135" s="30" t="n">
+        <v>130</v>
+      </c>
+      <c r="P135" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="Q135" s="33" t="n">
+        <v>201</v>
+      </c>
       <c r="R135" s="18" t="n">
         <f aca="false">AVERAGEIF($C135:$Q135,"&gt;0")</f>
-        <v>115.142857142857</v>
+        <v>126.545454545455</v>
       </c>
       <c r="U135" s="5" t="s">
         <v>213</v>
@@ -12848,6 +12861,9 @@
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>214</v>
+      </c>
+      <c r="B136" s="2" t="n">
+        <v>119</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
@@ -12949,14 +12965,14 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="n">
         <f aca="true">TODAY()</f>
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!B$3:B$159, "&gt;0")</f>
-        <v>116.557522123894</v>
+        <v>116.578947368421</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -13076,7 +13092,7 @@
       </c>
       <c r="C15" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!N$3:N$153, "&gt;0")</f>
-        <v>121.893617021277</v>
+        <v>122.0625</v>
       </c>
       <c r="D15" s="7"/>
     </row>
@@ -13086,7 +13102,7 @@
       </c>
       <c r="C16" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!O$3:O$153, "&gt;0")</f>
-        <v>126.261904761905</v>
+        <v>126.348837209302</v>
       </c>
       <c r="D16" s="7"/>
     </row>
@@ -13096,7 +13112,7 @@
       </c>
       <c r="C17" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!P$3:P$153, "&gt;0")</f>
-        <v>135.754385964912</v>
+        <v>135.568965517241</v>
       </c>
       <c r="D17" s="7"/>
     </row>
@@ -13106,7 +13122,7 @@
       </c>
       <c r="C18" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!Q$3:Q$159, "&gt;0")</f>
-        <v>122.949152542373</v>
+        <v>124.25</v>
       </c>
       <c r="D18" s="7"/>
     </row>

</xml_diff>

<commit_message>
Add "Bagging-Regressor-Example" to ptojects
</commit_message>
<xml_diff>
--- a/polynomial-trendlines/all-day-glucose.xlsx
+++ b/polynomial-trendlines/all-day-glucose.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="258">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -845,6 +845,41 @@
     <t xml:space="preserve">2024-03-26</t>
   </si>
   <si>
+    <t xml:space="preserve">9:20 AM: Weights, mostly 10x10; 7 PUs
+Lots of non-keto pasta for dinner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-03-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6:30 PM: Freestyle Libré. 6:40: 1 Voortman Choc Chip cookie (carbs, 12 gm). Glu rose to 160; -&gt;
+6:45: treadmill, 15m, 2.8 mph, 6%, 127 Cal, HR 120. Glu increase reversed abrupty; level dropped to 104 at 7:30.
+9 PM: Dinner. glu up to 161 before Irish Cream @ 9:30. 9: 35: Peak: 166.
+9:45: Treadmill, 20m, 2.5 mph, 5.5%, 140 Cal. Glu peaked at 202 ≈5 min after end.
+11:45 AM: Two isometric pull-ups. 12:11 AM: glu 134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-03-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 AM: 1 1/2 omelettes at Willows + coffee.
+10:55–11:10: Treadmill, 15m, 1.7 mph, 0%; glu:
+143–146; 150 at 11:15; 145 at 11:30 (no change)
+Unknown time: 7 PUs, Weights, 5&amp;10 x 10 reps;
+2 isometric pull-ups
+1:15–1:35: Pedal exerciser. Glu: 135 -&gt; 123.
+3:35: glu 140. 3:38: 2prunes. pedals, 8 m; glu -&gt; 126
+4 pm: 2 prunes + 1 Voortman, pedals 8 min, glu 131
+4:35 pm: pedals 10 min, glu:137-&gt;150
+5 PM high glu due to Voortman? Weight gain?
+5:50: Treadmill, 30 min, 2.8 mph, 6%; 247 Cal, HR 120
+Cream Whiskey with dinner. Glucose max 205 ca. 9:45 PM
+Home A1c: 7.0. 10 PM: Weights, mostly 10 lb, 10–20 reps. Glu -&gt; 122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-03-29</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -852,42 +887,313 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">9:20 AM: Weights, </t>
+      <t xml:space="preserve">7: 50: B’kfast w/ 5 blueberries. 8:10: 7 PUs, weights. 8: 25: glu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">197</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">mostly 10x10; 7 PUs
-Lots of non-keto pasta for dinner</t>
+      <t xml:space="preserve">.(Try exercises </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-03-27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6:30 PM: Freestyle Libré. 6:40: 1 Voortman Choc Chip cookie (carbs, 12 gm). Glu rose to 160; -&gt;
-6:45: treadmill, 15m, 2.8 mph, 6%, 127 Cal, HR 120. Glu increase reversed abrupty; level dropped to 104 at 7:30.
-9 PM: Dinner. glu up to 161 before Irish Cream @ 9:30. 9: 35: Peak: 166.
-9:45: Treadmill, 20m, 2.5 mph, 5.5%, 140 Cal. Glu peaked at 202 ≈5 min after end.
-11:45 AM: Two isometric pull-ups. 12:11 AM: glu 134</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-03-28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024-03-29</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">before</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> meals!)
+8:45: Glu seems level at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">145</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Pilates floor ex’s. Glu 105.
+12:25: lunch.1: 35: Glu seems to have peaked at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">145</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+Afternoon: pedal exerciser.—Hgb A1c from Parkview:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> 6.4.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8:25: Coffee whiskey.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">2024-03-30</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Ate during early AM; glu peaked at 160. 8: 35 AM: breakfast. Glu appears to have started rising (currently 149) 1/2 hour later. Seems to have peaked at 174.
+12 PM: Lunch: Chicken, tomatoes, 5 strawberries. Spike 1/2 hr later: max, 165.
+≈1:30 PM: Karen served me 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> lunch dozen grapes; Halo. Must spread the fruits out! Believe it peaked at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">165</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> again.
+8: 30 PM: Dinner; after-dinner Bourbon Cream. 9:15: Weights
+10 PM: The bump up to 139 is probably from the Bourbon Cream.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">2024-03-31</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8:30: Mushroom-spinach omelette w/hollandaise, IHOP
+10 AM: Treadmill, 30min, 2.8 mph, 6%; 247 cal, HR 138. Glu 125 
+8 PUs. —12 PM: Chin-up/Pull-up bar (”CUPU”).
+2:18: Pedals: glu 134, unimproved. Weights, 5 lb (15 min): glu dropped to 120.—3 PM: glu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">117</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> –&gt; 2 strawberries.—3:45: glu 132–&gt; weights, 5 lb, plus some floor. 3:57: glu 127. 4:10: 1 scrambled egg, 2 tomatoes, 1 pc. Karen’s “keto” date-nut bread. 4:35 PM: glu 134 –&gt; Pilates floor ex’s. 4:53: glu peaked </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">190, 4:54</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 6:30(?): Weights, selected.
+After dinner incl. Bourbon Cream glucose rose from 125 to 162. Treadmill: 30m, 2.4 mph, 5%; 132)?) Cal, HR 90. Glu dropped to 97 at 9:45, then rose to 115 –&gt; weights, 5 lbs –&gt; glu 108.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 AM: Glu: 119–135. Weights, 5 lb–&gt;glu ≈150. 8 AM: glu 140.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-04-30</t>
   </si>
   <si>
     <t xml:space="preserve">Hour</t>
@@ -920,7 +1226,7 @@
     <numFmt numFmtId="169" formatCode="#"/>
     <numFmt numFmtId="170" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -978,12 +1284,26 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1342,7 +1662,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart186.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart176.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1372,7 +1692,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.145465489566613"/>
+          <c:x val="0.14607869379015"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -1391,10 +1711,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.108346709470305"/>
-          <c:y val="0.168199554069119"/>
-          <c:w val="0.697498662386303"/>
-          <c:h val="0.542224080267559"/>
+          <c:x val="0.108404710920771"/>
+          <c:y val="0.168387276785714"/>
+          <c:w val="0.697336723768737"/>
+          <c:h val="0.541713169642857"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1524,9 +1844,9 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'all-day-glucose'!$A$3:$A$140</c:f>
+              <c:f>'all-day-glucose'!$A$3:$A$170</c:f>
               <c:strCache>
-                <c:ptCount val="138"/>
+                <c:ptCount val="168"/>
                 <c:pt idx="0">
                   <c:v>2023-11-08</c:v>
                 </c:pt>
@@ -1940,16 +2260,106 @@
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>2024-04-01</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2024-04-02</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2024-04-03</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2024-04-04</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2024-04-05</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2024-04-06</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2024-04-07</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2024-04-08</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2024-04-09</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>2024-04-10</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2024-04-11</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2024-04-12</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2024-04-13</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2024-04-14</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2024-04-15</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2024-04-16</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2024-04-17</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2024-04-18</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2024-04-19</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2024-04-20</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2024-04-21</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2024-04-22</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2024-04-23</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2024-04-24</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2024-04-25</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2024-04-26</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2024-04-27</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>2024-04-28</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2024-04-29</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2024-04-30</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'all-day-glucose'!$R$3:$R$140</c:f>
+              <c:f>'all-day-glucose'!$R$3:$R$170</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="138"/>
+                <c:ptCount val="168"/>
                 <c:pt idx="0">
                   <c:v>124.5</c:v>
                 </c:pt>
@@ -2324,6 +2734,21 @@
                 </c:pt>
                 <c:pt idx="132">
                   <c:v>126.545454545455</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>137.416666666667</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>127.222222222222</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>133.133333333333</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>135.2</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2338,11 +2763,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="32662322"/>
-        <c:axId val="1573105"/>
+        <c:axId val="50533348"/>
+        <c:axId val="85260864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="32662322"/>
+        <c:axId val="50533348"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2370,7 +2795,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1573105"/>
+        <c:crossAx val="85260864"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2378,7 +2803,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1573105"/>
+        <c:axId val="85260864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="155"/>
@@ -2419,8 +2844,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.021669341894061"/>
-              <c:y val="0.204849498327759"/>
+              <c:x val="0.0216809421841542"/>
+              <c:y val="0.202845982142857"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2453,7 +2878,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32662322"/>
+        <c:crossAx val="50533348"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -2515,7 +2940,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart187.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart177.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2545,7 +2970,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.228302658486708"/>
+          <c:x val="0.228452156830646"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -2564,10 +2989,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101840490797546"/>
-          <c:y val="0.188308977035491"/>
-          <c:w val="0.656850715746421"/>
-          <c:h val="0.492553931802366"/>
+          <c:x val="0.101907178521732"/>
+          <c:y val="0.188518879754772"/>
+          <c:w val="0.656626012932799"/>
+          <c:h val="0.491988295945381"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2697,9 +3122,9 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'all-day-glucose'!$A$3:$A$140</c:f>
+              <c:f>'all-day-glucose'!$A$3:$A$170</c:f>
               <c:strCache>
-                <c:ptCount val="138"/>
+                <c:ptCount val="168"/>
                 <c:pt idx="0">
                   <c:v>2023-11-08</c:v>
                 </c:pt>
@@ -3113,16 +3538,106 @@
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>2024-04-01</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2024-04-02</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2024-04-03</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2024-04-04</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2024-04-05</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2024-04-06</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2024-04-07</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2024-04-08</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2024-04-09</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>2024-04-10</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2024-04-11</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2024-04-12</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2024-04-13</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2024-04-14</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2024-04-15</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2024-04-16</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2024-04-17</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2024-04-18</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2024-04-19</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2024-04-20</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>2024-04-21</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>2024-04-22</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2024-04-23</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2024-04-24</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>2024-04-25</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>2024-04-26</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2024-04-27</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>2024-04-28</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2024-04-29</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>2024-04-30</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'all-day-glucose'!$B$3:$B$140</c:f>
+              <c:f>'all-day-glucose'!$B$3:$B$170</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="138"/>
+                <c:ptCount val="168"/>
                 <c:pt idx="1">
                   <c:v>104</c:v>
                 </c:pt>
@@ -3463,6 +3978,15 @@
                   <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="133">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="137">
                   <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
@@ -3478,11 +4002,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="87844347"/>
-        <c:axId val="56868977"/>
+        <c:axId val="61572794"/>
+        <c:axId val="35731499"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87844347"/>
+        <c:axId val="61572794"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3510,7 +4034,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56868977"/>
+        <c:crossAx val="35731499"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3518,7 +4042,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56868977"/>
+        <c:axId val="35731499"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -3557,7 +4081,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87844347"/>
+        <c:crossAx val="61572794"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -3619,7 +4143,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart188.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart178.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3659,10 +4183,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.138631168481915"/>
-          <c:y val="0.177078718062325"/>
-          <c:w val="0.706871050154632"/>
-          <c:h val="0.539506719834589"/>
+          <c:x val="0.138705771559263"/>
+          <c:y val="0.177288185716398"/>
+          <c:w val="0.706713305529396"/>
+          <c:h val="0.53896199911282"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3781,52 +4305,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>116.578947368421</c:v>
+                  <c:v>116.786324786325</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>130.064516129032</c:v>
+                  <c:v>131.114285714286</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136.163265306122</c:v>
+                  <c:v>136.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>125.66</c:v>
+                  <c:v>126.384615384615</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>127.392156862745</c:v>
+                  <c:v>128.036363636364</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>117.962962962963</c:v>
+                  <c:v>118.754385964912</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>133.22</c:v>
+                  <c:v>133.759259259259</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>125.782608695652</c:v>
+                  <c:v>126.163265306122</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130.181818181818</c:v>
+                  <c:v>130.391304347826</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>125.240740740741</c:v>
+                  <c:v>125.017543859649</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>123.684210526316</c:v>
+                  <c:v>125.032786885246</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>126.4375</c:v>
+                  <c:v>126.096153846154</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>122.0625</c:v>
+                  <c:v>121.730769230769</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>126.348837209302</c:v>
+                  <c:v>125.68085106383</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>135.568965517241</c:v>
+                  <c:v>136.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>124.25</c:v>
+                  <c:v>124.734375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3834,11 +4358,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="90558165"/>
-        <c:axId val="73345214"/>
+        <c:axId val="58635153"/>
+        <c:axId val="36030426"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="90558165"/>
+        <c:axId val="58635153"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3868,8 +4392,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.400968132311416"/>
-              <c:y val="0.892334957908728"/>
+              <c:x val="0.400645768868559"/>
+              <c:y val="0.892207600177436"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3902,7 +4426,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73345214"/>
+        <c:crossAx val="36030426"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3910,7 +4434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73345214"/>
+        <c:axId val="36030426"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="110"/>
@@ -3976,7 +4500,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90558165"/>
+        <c:crossAx val="58635153"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4027,7 +4551,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart189.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart179.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4057,7 +4581,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.181828791503764"/>
+          <c:x val="0.182380757779205"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -4076,10 +4600,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.094182178911128"/>
-          <c:y val="0.134916519755263"/>
-          <c:w val="0.707358347435374"/>
-          <c:h val="0.664212382038785"/>
+          <c:x val="0.094226166150972"/>
+          <c:y val="0.135028541774779"/>
+          <c:w val="0.707221670850604"/>
+          <c:h val="0.663933575505968"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4948,11 +5472,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="84820420"/>
-        <c:axId val="41054328"/>
+        <c:axId val="6906432"/>
+        <c:axId val="2982138"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="84820420"/>
+        <c:axId val="6906432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45413"/>
@@ -4982,7 +5506,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41054328"/>
+        <c:crossAx val="2982138"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -4992,7 +5516,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="41054328"/>
+        <c:axId val="2982138"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -5031,7 +5555,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84820420"/>
+        <c:crossAx val="6906432"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -5096,7 +5620,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart190.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart180.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5125,8 +5649,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.192689477986687"/>
-          <c:y val="0.00937081659973226"/>
+          <c:x val="0.192779530318963"/>
+          <c:y val="0.00938086303939963"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5144,10 +5668,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.104694616372767"/>
-          <c:y val="0.114859437751004"/>
-          <c:w val="0.64410837323368"/>
-          <c:h val="0.626773761713521"/>
+          <c:x val="0.104743544806636"/>
+          <c:y val="0.114982578397213"/>
+          <c:w val="0.643942049304825"/>
+          <c:h val="0.626373626373626"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -7108,11 +7632,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="38087513"/>
-        <c:axId val="57775575"/>
+        <c:axId val="54033705"/>
+        <c:axId val="99650762"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="38087513"/>
+        <c:axId val="54033705"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7140,7 +7664,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57775575"/>
+        <c:crossAx val="99650762"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7148,7 +7672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57775575"/>
+        <c:axId val="99650762"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -7187,7 +7711,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38087513"/>
+        <c:crossAx val="54033705"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -7263,9 +7787,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>273240</xdr:colOff>
+      <xdr:colOff>270360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2667240</xdr:rowOff>
+      <xdr:rowOff>2664360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7274,7 +7798,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="90360" y="84240"/>
-        <a:ext cx="5382360" cy="2583000"/>
+        <a:ext cx="5379480" cy="2580120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7293,9 +7817,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>2733840</xdr:colOff>
+      <xdr:colOff>2730960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2682720</xdr:rowOff>
+      <xdr:rowOff>2679840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7304,7 +7828,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5563440" y="96480"/>
-        <a:ext cx="4400640" cy="2586240"/>
+        <a:ext cx="4397760" cy="2583360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7328,9 +7852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>755640</xdr:colOff>
+      <xdr:colOff>752760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2490120</xdr:rowOff>
+      <xdr:rowOff>2487240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7339,7 +7863,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="42120" y="52920"/>
-        <a:ext cx="5354280" cy="2437200"/>
+        <a:ext cx="5351400" cy="2434320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7363,9 +7887,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>524880</xdr:colOff>
+      <xdr:colOff>522000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>105480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7374,7 +7898,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="45360" y="51120"/>
-        <a:ext cx="6168960" cy="3471120"/>
+        <a:ext cx="6166080" cy="3468240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7393,9 +7917,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>529200</xdr:colOff>
+      <xdr:colOff>526320</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>106920</xdr:rowOff>
+      <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7404,7 +7928,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="53640" y="3595320"/>
-        <a:ext cx="6165000" cy="2688840"/>
+        <a:ext cx="6162120" cy="2685960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7422,12 +7946,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM140"/>
+  <dimension ref="A1:AM169"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4532" topLeftCell="C133" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="4253" topLeftCell="C139" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C136" activeCellId="0" sqref="C136"/>
+      <selection pane="bottomLeft" activeCell="B142" activeCellId="0" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7452,7 +7976,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="9.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="8.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="4" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="5" width="39.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="5" width="45.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="4.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="7" width="2.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="7" width="2.82"/>
@@ -7643,6 +8167,7 @@
         <f aca="false">AVERAGEIF($C$4:$Q$4, "&gt;0")</f>
         <v>118.75</v>
       </c>
+      <c r="S4" s="19"/>
       <c r="U4" s="21"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12806,7 +13331,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="134.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="101.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>212</v>
       </c>
@@ -12858,50 +13383,456 @@
         <v>213</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="156.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
         <v>214</v>
       </c>
       <c r="B136" s="2" t="n">
         <v>119</v>
       </c>
-      <c r="C136" s="2"/>
+      <c r="C136" s="2" t="n">
+        <v>135</v>
+      </c>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
-      <c r="F136" s="2"/>
-      <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
-      <c r="I136" s="30" t="s">
+      <c r="F136" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="G136" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="H136" s="2" t="n">
+        <v>134</v>
+      </c>
+      <c r="I136" s="30" t="n">
+        <v>123</v>
+      </c>
+      <c r="J136" s="2"/>
+      <c r="K136" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="L136" s="32" t="n">
+        <v>162</v>
+      </c>
+      <c r="M136" s="2" t="n">
+        <v>129</v>
+      </c>
+      <c r="N136" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="O136" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="P136" s="32" t="n">
+        <v>193</v>
+      </c>
+      <c r="Q136" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="R136" s="18" t="n">
+        <f aca="false">AVERAGEIF($C136:$Q136,"&gt;0")</f>
+        <v>137.416666666667</v>
+      </c>
+      <c r="U136" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="67.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B137" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="C137" s="30" t="n">
+        <v>145</v>
+      </c>
+      <c r="D137" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2" t="n">
+        <v>133</v>
+      </c>
+      <c r="I137" s="2"/>
+      <c r="J137" s="30"/>
+      <c r="K137" s="2"/>
+      <c r="L137" s="2" t="n">
+        <v>131</v>
+      </c>
+      <c r="M137" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="N137" s="2" t="n">
+        <v>121</v>
+      </c>
+      <c r="O137" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="P137" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="Q137" s="30" t="n">
+        <v>135</v>
+      </c>
+      <c r="R137" s="18" t="n">
+        <f aca="false">AVERAGEIF($C137:$Q137,"&gt;0")</f>
+        <v>127.222222222222</v>
+      </c>
+      <c r="U137" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="101.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C138" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="D138" s="32" t="n">
+        <v>152</v>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>121</v>
+      </c>
+      <c r="F138" s="2" t="n">
+        <v>131</v>
+      </c>
+      <c r="G138" s="2" t="n">
+        <v>126</v>
+      </c>
+      <c r="H138" s="32" t="n">
+        <v>161</v>
+      </c>
+      <c r="I138" s="2" t="n">
+        <v>140</v>
+      </c>
+      <c r="J138" s="32" t="n">
+        <v>153</v>
+      </c>
+      <c r="K138" s="30" t="n">
+        <v>119</v>
+      </c>
+      <c r="L138" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="M138" s="2" t="n">
+        <v>124</v>
+      </c>
+      <c r="N138" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="O138" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="P138" s="2" t="n">
+        <v>139</v>
+      </c>
+      <c r="Q138" s="2" t="n">
+        <v>140</v>
+      </c>
+      <c r="R138" s="18" t="n">
+        <f aca="false">AVERAGEIF($C138:$Q138,"&gt;0")</f>
+        <v>133.133333333333</v>
+      </c>
+      <c r="U138" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="167.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B139" s="2" t="n">
+        <v>135</v>
+      </c>
+      <c r="C139" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="D139" s="32" t="n">
+        <v>162</v>
+      </c>
+      <c r="E139" s="32" t="n">
+        <v>168</v>
+      </c>
+      <c r="F139" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="G139" s="2" t="n">
+        <v>136</v>
+      </c>
+      <c r="H139" s="2" t="n">
+        <v>134</v>
+      </c>
+      <c r="I139" s="2" t="n">
+        <v>133</v>
+      </c>
+      <c r="J139" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="K139" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="L139" s="32" t="n">
+        <v>169</v>
+      </c>
+      <c r="M139" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="N139" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="O139" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="P139" s="32" t="n">
+        <v>152</v>
+      </c>
+      <c r="Q139" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="R139" s="18" t="n">
+        <f aca="false">AVERAGEIF($C139:$Q139,"&gt;0")</f>
+        <v>135.2</v>
+      </c>
+      <c r="U139" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B140" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="30" t="n">
+        <v>139</v>
+      </c>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="J136" s="2"/>
-      <c r="K136" s="2"/>
-      <c r="L136" s="2"/>
-      <c r="M136" s="2"/>
-      <c r="N136" s="2"/>
-      <c r="P136" s="30" t="s">
+      <c r="N140" s="2"/>
+      <c r="P140" s="2"/>
+      <c r="Q140" s="2"/>
+      <c r="R140" s="18" t="n">
+        <f aca="false">AVERAGEIF($C140:$Q140,"&gt;0")</f>
+        <v>139</v>
+      </c>
+      <c r="U140" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="Q136" s="2"/>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="s">
-        <v>218</v>
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+      <c r="J141" s="2"/>
+      <c r="K141" s="2"/>
+      <c r="L141" s="2"/>
+      <c r="M141" s="2"/>
+      <c r="N141" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P141" s="2"/>
+      <c r="Q141" s="2"/>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C142" s="2"/>
+      <c r="D142" s="2"/>
+      <c r="E142" s="2"/>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+      <c r="H142" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I142" s="2"/>
+      <c r="J142" s="2"/>
+      <c r="K142" s="2"/>
+      <c r="L142" s="2"/>
+      <c r="M142" s="2"/>
+      <c r="N142" s="2"/>
+      <c r="O142" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P142" s="2"/>
+      <c r="Q142" s="2"/>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C143" s="2"/>
+      <c r="D143" s="2"/>
+      <c r="E143" s="2"/>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+      <c r="H143" s="2"/>
+      <c r="I143" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="J143" s="2"/>
+      <c r="K143" s="2"/>
+      <c r="L143" s="2"/>
+      <c r="M143" s="2"/>
+      <c r="N143" s="2"/>
+      <c r="P143" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q143" s="2"/>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -12955,24 +13886,24 @@
         <v>0</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>219</v>
+        <v>253</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>220</v>
+        <v>254</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="n">
         <f aca="true">TODAY()</f>
-        <v>45379</v>
+        <v>45383</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!B$3:B$159, "&gt;0")</f>
-        <v>116.578947368421</v>
+        <v>116.786324786325</v>
       </c>
       <c r="D3" s="7"/>
     </row>
@@ -12982,7 +13913,7 @@
       </c>
       <c r="C4" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!C$3:C$153, "&gt;0")</f>
-        <v>130.064516129032</v>
+        <v>131.114285714286</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -12992,7 +13923,7 @@
       </c>
       <c r="C5" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!D$3:D$153, "&gt;0")</f>
-        <v>136.163265306122</v>
+        <v>136.75</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -13002,7 +13933,7 @@
       </c>
       <c r="C6" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!E$3:E$153, "&gt;0")</f>
-        <v>125.66</v>
+        <v>126.384615384615</v>
       </c>
       <c r="D6" s="7"/>
     </row>
@@ -13012,7 +13943,7 @@
       </c>
       <c r="C7" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!F$3:F$153, "&gt;0")</f>
-        <v>127.392156862745</v>
+        <v>128.036363636364</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -13022,7 +13953,7 @@
       </c>
       <c r="C8" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!G$3:G$153, "&gt;0")</f>
-        <v>117.962962962963</v>
+        <v>118.754385964912</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -13032,7 +13963,7 @@
       </c>
       <c r="C9" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!H$3:H$153, "&gt;0")</f>
-        <v>133.22</v>
+        <v>133.759259259259</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -13042,7 +13973,7 @@
       </c>
       <c r="C10" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!I$3:I$153, "&gt;0")</f>
-        <v>125.782608695652</v>
+        <v>126.163265306122</v>
       </c>
       <c r="D10" s="7"/>
     </row>
@@ -13052,7 +13983,7 @@
       </c>
       <c r="C11" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!J$3:J$153, "&gt;0")</f>
-        <v>130.181818181818</v>
+        <v>130.391304347826</v>
       </c>
       <c r="D11" s="7"/>
     </row>
@@ -13062,7 +13993,7 @@
       </c>
       <c r="C12" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!K$3:K$153, "&gt;0")</f>
-        <v>125.240740740741</v>
+        <v>125.017543859649</v>
       </c>
       <c r="D12" s="7"/>
     </row>
@@ -13072,7 +14003,7 @@
       </c>
       <c r="C13" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!L$3:L$153, "&gt;0")</f>
-        <v>123.684210526316</v>
+        <v>125.032786885246</v>
       </c>
       <c r="D13" s="7"/>
     </row>
@@ -13082,7 +14013,7 @@
       </c>
       <c r="C14" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!M$3:M$153, "&gt;0")</f>
-        <v>126.4375</v>
+        <v>126.096153846154</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -13092,7 +14023,7 @@
       </c>
       <c r="C15" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!N$3:N$153, "&gt;0")</f>
-        <v>122.0625</v>
+        <v>121.730769230769</v>
       </c>
       <c r="D15" s="7"/>
     </row>
@@ -13102,7 +14033,7 @@
       </c>
       <c r="C16" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!O$3:O$153, "&gt;0")</f>
-        <v>126.348837209302</v>
+        <v>125.68085106383</v>
       </c>
       <c r="D16" s="7"/>
     </row>
@@ -13112,7 +14043,7 @@
       </c>
       <c r="C17" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!P$3:P$153, "&gt;0")</f>
-        <v>135.568965517241</v>
+        <v>136.5</v>
       </c>
       <c r="D17" s="7"/>
     </row>
@@ -13122,7 +14053,7 @@
       </c>
       <c r="C18" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!Q$3:Q$159, "&gt;0")</f>
-        <v>124.25</v>
+        <v>124.734375</v>
       </c>
       <c r="D18" s="7"/>
     </row>
@@ -13141,7 +14072,7 @@
         <v>10</v>
       </c>
       <c r="U95" s="7" t="s">
-        <v>221</v>
+        <v>255</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13159,7 +14090,7 @@
         <v>117</v>
       </c>
       <c r="U113" s="49" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13221,7 +14152,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="E1" s="2" t="n">
         <v>0</v>
@@ -13268,7 +14199,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
@@ -13315,7 +14246,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -13362,7 +14293,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>0</v>
@@ -13409,7 +14340,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>0</v>
@@ -13456,7 +14387,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0</v>
@@ -13503,7 +14434,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Added unpushed changes from A1c, Braided-Lissajous-Curve, polynomial-trendlines, transcript_scraper
</commit_message>
<xml_diff>
--- a/polynomial-trendlines/all-day-glucose.xlsx
+++ b/polynomial-trendlines/all-day-glucose.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="369">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -1106,18 +1106,410 @@
     <t xml:space="preserve">2024-04-01</t>
   </si>
   <si>
-    <t xml:space="preserve">7 AM: Glu: 119–135. Weights, 5 lb–&gt;glu ≈150. 8 AM: glu 140.</t>
+    <t xml:space="preserve">7 AM: Glu: 119–135. Weights, 5 lb–&gt;glu ≈150. 8 AM: glu 140. 1 PM: glu 127; lunch (deviled eggs minus olives), peach tea and two strawberries.) CUPU. 8 PUs (skip tomorrow.) Two more strawberries. – 3:50 PM: two more strawberries. – ≈ 5 PM: two strawberries
+5:30 PM: Ice cream sandwich: carbs=26 gm; glu 115.
+6 PM glucose rise began. Peaked at 168, 6:30–6:40.
+7 PM: Dinner: Atkins Beef Merlot. 7:20: Bourbon Cream. Glu: 141 –&gt; ( rise started 8 PM.) 8:30: CUPU. Very small bump: 125 –&gt; 130.</t>
   </si>
   <si>
     <t xml:space="preserve">2024-04-02</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">7:30 AM: Weights, mostly 10 lb, 10 reps. Glucose increased. – 8:30: b’kfast incl 5 raspberries Post bkfast peak: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">170</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> ca. 8:45. Dropped to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">123</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> by 10:30.
+5 PM: 4 Tea Cookies. Glu: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">118</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> –&gt; rise starting 5:20 to 152. — 6:12–6:25: Weights, 5&amp;10 lbs, 10 reps. Peak: 6:30. — 6:45: No decrease. Effect of Pukka Tea? (Has “berries”.) (No calories.) Effect of cheese? Peak, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">159</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, at 7 PM. Dinner: ?? 8:30 PM. 9PM abrupt rise in glucose; peaked at ≈ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">160</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> at 10 PM. Nadir: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">113</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, 11 PM</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-03</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">7 AM: 8 PUs, weights 10 lbs, 10 reps
+1:24 PM: Glucose = 142 -&gt; treadmill, 20m x 2 mph x 2%, 90 Cal. HR peak: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">152</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, came back to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">147</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Finished ≈ 1:50.
+Glucose rose to 187 at ≈ 2:50. (Had 5 tea cookies and Karen’s keto bread.)
+7 PM: glu 117. More keto bread. Glu peaked at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">152</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, but there was also dinner.
+9 PM: glucose </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. 9:10: Irish Cream. 9:20: rapid rise to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">173</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. I got on the treadmill when glucose was ≈170. Treadmill: 30 min, 2.8 mph, 4%; 200 Cal, HR 102. Glucose came down to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">75</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, then came back up. Currently stable(?) at 109.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-04</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">7 AM: glucose rose to 130+ before bkfast (granola, 6 raspberries, V-8, coffee w/low-carb milk.) Glu rose to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">160</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> –&gt; treadmill, 28’, 2mph, 2–4%; 100 Cal.) Max glu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">164</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; began descending after 12 min; fell to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">128</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; after ex. over fell further to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF00A933"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">116</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+12 PM: glu 142 –&gt; treadmill, 26m, 1.5–2 mph; 2, 3, 4 %; 145 Cal. Glu rose to 143, then dropped to 129 (subsequent drop of 3) suggests 10 Cal/mg; 16 min/14 mg (plus 10 minutes startup). CUPU
+After </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Apple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Walnut salad, glucose spiked to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF8000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">177</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.
+3:50 PM: Miso soup. Glu 117. 4:30: No change. 
+4:40: Chinese noodles. Glu 107. 5:05: started up. 5:15: 128. Treadmill, 45 min, 2–2.5 mph, 2–4.5%. 300 Cal, HR 90. Glu peaked at 148, 10 min into exercise; came down slowly to 122 and hung (effect of noodles dinner?)6:50: coffee liqueur.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-05</t>
   </si>
   <si>
@@ -1127,12 +1519,33 @@
     <t xml:space="preserve">2024-04-07</t>
   </si>
   <si>
+    <t xml:space="preserve">9: 40 AM: Glu185.Ex–&gt;glu 120
+11:20 AM: Glu 143. Ex-&gt; glu 120
+12:10(?) Lunch: glu 131
+3 PM: glu 122. 1 orange slice. Glu peaked at 135.
+Avg. glucose 130 ~ A1c 6.2.
+4 PM: glu 117, 1 orange slice; peak glu 135 
+6 PM: glu 120, 1 orange slice
+7 PM: glu 125, 1 orange slice
+8:30 PM: Dinner; Glu: 125 –&gt; 165.
+9:30 PM: Exercise, ≈50 min, 2–2.7 mph, 4–9%. 469  Cal, HR 120. Glu –&gt; 105.</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-08</t>
   </si>
   <si>
+    <t xml:space="preserve">8: 45 AM: breakfast. Glu 135</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-09</t>
   </si>
   <si>
+    <t xml:space="preserve">10 AM: bkfast at Tony’s: glu up to 150.
+11:10: V-8. Glu: 130 –&gt;128
+7 PM: 9 PUs. 
+10:10 PM: Coffee, shotglass Irish Cream. Glu: 107–&gt;127</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-10</t>
   </si>
   <si>
@@ -1148,6 +1561,9 @@
     <t xml:space="preserve">2024-04-14</t>
   </si>
   <si>
+    <t xml:space="preserve">Ozempic 0.25 mg</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-15</t>
   </si>
   <si>
@@ -1163,6 +1579,9 @@
     <t xml:space="preserve">2024-04-19</t>
   </si>
   <si>
+    <t xml:space="preserve">Treadmill: 30 min, 1.5–2.4mph, 4–9%.—10 PUs.</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-20</t>
   </si>
   <si>
@@ -1175,6 +1594,9 @@
     <t xml:space="preserve">2024-04-23</t>
   </si>
   <si>
+    <t xml:space="preserve">PUs: 11</t>
+  </si>
+  <si>
     <t xml:space="preserve">2024-04-24</t>
   </si>
   <si>
@@ -1194,6 +1616,312 @@
   </si>
   <si>
     <t xml:space="preserve">2024-04-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ozempic 0.5 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUs: 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Ozempic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUs: 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUs: 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-05-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ozempic 0.33 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUs: 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ozempic 1 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUs: 12+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-06-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ozempic 1 mg; PUs: 13+4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024-07-31</t>
   </si>
   <si>
     <t xml:space="preserve">Hour</t>
@@ -1298,12 +2026,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1389,7 +2117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1474,7 +2202,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1554,6 +2282,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1627,7 +2359,7 @@
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFE6E905"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -1662,7 +2394,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart176.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1683,7 +2415,7 @@
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Average Glucose by Date (Non-Fasting)
-(Polynomial trendline degrees 1–4)</a:t>
+(Polynomial trendline degrees 1–3)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1692,7 +2424,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14607869379015"/>
+          <c:x val="0.147726511752494"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -1711,10 +2443,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.108404710920771"/>
-          <c:y val="0.168387276785714"/>
-          <c:w val="0.697336723768737"/>
-          <c:h val="0.541713169642857"/>
+          <c:x val="0.108283667046139"/>
+          <c:y val="0.188851792713021"/>
+          <c:w val="0.696243219714726"/>
+          <c:h val="0.542168674698795"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1736,12 +2468,13 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
-            <a:ln w="0">
+            <a:ln w="27360">
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -1809,24 +2542,6 @@
             <c:dispEq val="0"/>
           </c:trendline>
           <c:trendline>
-            <c:name>Degree 4</c:name>
-            <c:spPr>
-              <a:ln w="18360">
-                <a:solidFill>
-                  <a:srgbClr val="ffff00"/>
-                </a:solidFill>
-                <a:prstDash val="dash"/>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="4"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
             <c:name>Linear</c:name>
             <c:spPr>
               <a:ln w="18360">
@@ -2349,7 +3064,7 @@
                   <c:v>2024-04-30</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v/>
+                  <c:v>2024-05-01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2748,7 +3463,25 @@
                   <c:v>135.2</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>139</c:v>
+                  <c:v>129.928571428571</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>137.333333333333</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>134.133333333333</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>129.4</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2763,11 +3496,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="50533348"/>
-        <c:axId val="85260864"/>
+        <c:axId val="45184396"/>
+        <c:axId val="35321056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50533348"/>
+        <c:axId val="45184396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2785,7 +3518,7 @@
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-3600000"/>
+          <a:bodyPr rot="-2700000"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2795,7 +3528,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="85260864"/>
+        <c:crossAx val="35321056"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2803,7 +3536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85260864"/>
+        <c:axId val="35321056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="155"/>
@@ -2844,8 +3577,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0216809421841542"/>
-              <c:y val="0.202845982142857"/>
+              <c:x val="0.0217638786580058"/>
+              <c:y val="0.196835534910727"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2878,7 +3611,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50533348"/>
+        <c:crossAx val="45184396"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -2902,7 +3635,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.815641711229947"/>
-          <c:y val="0.141154742697373"/>
+          <c:y val="0.190659693192423"/>
           <c:w val="0.171256684491979"/>
           <c:h val="0.540924276169265"/>
         </c:manualLayout>
@@ -2940,7 +3673,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart177.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2961,7 +3694,7 @@
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>FBS by Date
-(Trendline degrees 1–4)</a:t>
+(Trendline degrees 1–3)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2970,7 +3703,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.228452156830646"/>
+          <c:x val="0.228683757883529"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -2989,10 +3722,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101907178521732"/>
-          <c:y val="0.188518879754772"/>
-          <c:w val="0.656626012932799"/>
-          <c:h val="0.491988295945381"/>
+          <c:x val="0.118519125235482"/>
+          <c:y val="0.18919312554617"/>
+          <c:w val="0.638791055778524"/>
+          <c:h val="0.54675211185552"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3014,12 +3747,13 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="004586"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
-            <a:ln w="0">
+            <a:ln w="27360">
               <a:solidFill>
-                <a:srgbClr val="004586"/>
+                <a:srgbClr val="000000"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -3087,24 +3821,6 @@
             <c:dispEq val="0"/>
           </c:trendline>
           <c:trendline>
-            <c:name>Degree 4</c:name>
-            <c:spPr>
-              <a:ln cap="rnd" w="18360">
-                <a:solidFill>
-                  <a:srgbClr val="e6e905"/>
-                </a:solidFill>
-                <a:prstDash val="dash"/>
-                <a:round/>
-              </a:ln>
-            </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="4"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
             <c:name>Linear</c:name>
             <c:spPr>
               <a:ln w="18360">
@@ -3627,7 +4343,7 @@
                   <c:v>2024-04-30</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v/>
+                  <c:v>2024-05-01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3988,6 +4704,36 @@
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4002,11 +4748,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="61572794"/>
-        <c:axId val="35731499"/>
+        <c:axId val="61302322"/>
+        <c:axId val="7213877"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61572794"/>
+        <c:axId val="61302322"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4024,7 +4770,7 @@
           </a:ln>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5100000"/>
+          <a:bodyPr rot="-2700000"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4034,7 +4780,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="35731499"/>
+        <c:crossAx val="7213877"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4042,7 +4788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35731499"/>
+        <c:axId val="7213877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -4081,7 +4827,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61572794"/>
+        <c:crossAx val="61302322"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -4143,7 +4889,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart178.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4183,10 +4929,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.138705771559263"/>
-          <c:y val="0.177288185716398"/>
-          <c:w val="0.706713305529396"/>
-          <c:h val="0.53896199911282"/>
+          <c:x val="0.138911290322581"/>
+          <c:y val="0.177893175074184"/>
+          <c:w val="0.706182795698925"/>
+          <c:h val="0.537388724035608"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -4305,52 +5051,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>116.786324786325</c:v>
+                  <c:v>116.92125984252</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>131.114285714286</c:v>
+                  <c:v>132.857142857143</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136.75</c:v>
+                  <c:v>136.736842105263</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>126.384615384615</c:v>
+                  <c:v>126.964912280702</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>128.036363636364</c:v>
+                  <c:v>128.64406779661</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118.754385964912</c:v>
+                  <c:v>120.693548387097</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>133.759259259259</c:v>
+                  <c:v>133.672413793103</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>126.163265306122</c:v>
+                  <c:v>126.924528301887</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130.391304347826</c:v>
+                  <c:v>130.372549019608</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>125.017543859649</c:v>
+                  <c:v>124.338709677419</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>125.032786885246</c:v>
+                  <c:v>124.242424242424</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>126.096153846154</c:v>
+                  <c:v>126.293103448276</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>121.730769230769</c:v>
+                  <c:v>122.859649122807</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>125.68085106383</c:v>
+                  <c:v>126.377358490566</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>136.5</c:v>
+                  <c:v>135.102941176471</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>124.734375</c:v>
+                  <c:v>125.728571428571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4358,11 +5104,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="58635153"/>
-        <c:axId val="36030426"/>
+        <c:axId val="96544912"/>
+        <c:axId val="11050006"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="58635153"/>
+        <c:axId val="96544912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4392,8 +5138,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.400645768868559"/>
-              <c:y val="0.892207600177436"/>
+              <c:x val="0.399731182795699"/>
+              <c:y val="0.891839762611276"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4426,7 +5172,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36030426"/>
+        <c:crossAx val="11050006"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4434,7 +5180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36030426"/>
+        <c:axId val="11050006"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="110"/>
@@ -4500,7 +5246,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="58635153"/>
+        <c:crossAx val="96544912"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4551,7 +5297,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart179.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4581,7 +5327,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.182380757779205"/>
+          <c:x val="0.183841906422552"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -4600,10 +5346,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.094226166150972"/>
-          <c:y val="0.135028541774779"/>
-          <c:w val="0.707221670850604"/>
-          <c:h val="0.663933575505968"/>
+          <c:x val="0.0942749200813717"/>
+          <c:y val="0.13535164377861"/>
+          <c:w val="0.706713164777681"/>
+          <c:h val="0.663129421556388"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5472,11 +6218,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6906432"/>
-        <c:axId val="2982138"/>
+        <c:axId val="40954000"/>
+        <c:axId val="60753358"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="6906432"/>
+        <c:axId val="40954000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45413"/>
@@ -5506,7 +6252,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2982138"/>
+        <c:crossAx val="60753358"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -5516,7 +6262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2982138"/>
+        <c:axId val="60753358"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -5555,7 +6301,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6906432"/>
+        <c:crossAx val="40954000"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -5620,7 +6366,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart180.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5649,8 +6395,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.192779530318963"/>
-          <c:y val="0.00938086303939963"/>
+          <c:x val="0.19285797371176"/>
+          <c:y val="0.00940986691759645"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5668,10 +6414,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.104743544806636"/>
-          <c:y val="0.114982578397213"/>
-          <c:w val="0.643942049304825"/>
-          <c:h val="0.626373626373626"/>
+          <c:x val="0.104745841572642"/>
+          <c:y val="0.115338083075682"/>
+          <c:w val="0.643422123996743"/>
+          <c:h val="0.625218443339158"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -7632,11 +8378,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="54033705"/>
-        <c:axId val="99650762"/>
+        <c:axId val="79692514"/>
+        <c:axId val="34176871"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54033705"/>
+        <c:axId val="79692514"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7664,7 +8410,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99650762"/>
+        <c:crossAx val="34176871"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7672,7 +8418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99650762"/>
+        <c:axId val="34176871"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -7711,7 +8457,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="54033705"/>
+        <c:crossAx val="79692514"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -7781,15 +8527,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>90360</xdr:colOff>
+      <xdr:colOff>92520</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>84240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>270360</xdr:colOff>
+      <xdr:colOff>263520</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2664360</xdr:rowOff>
+      <xdr:rowOff>2563920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7797,8 +8543,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="90360" y="84240"/>
-        <a:ext cx="5379480" cy="2580120"/>
+        <a:off x="92520" y="84240"/>
+        <a:ext cx="5375520" cy="2479680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7811,15 +8557,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>25560</xdr:colOff>
+      <xdr:colOff>23760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>92520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>2730960</xdr:colOff>
+      <xdr:colOff>2725560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2679840</xdr:rowOff>
+      <xdr:rowOff>2563920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7827,8 +8573,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5563440" y="96480"/>
-        <a:ext cx="4397760" cy="2583360"/>
+        <a:off x="5566680" y="92520"/>
+        <a:ext cx="4394880" cy="2471400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7852,9 +8598,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>752760</xdr:colOff>
+      <xdr:colOff>744480</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2487240</xdr:rowOff>
+      <xdr:rowOff>2478960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7863,7 +8609,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="42120" y="52920"/>
-        <a:ext cx="5351400" cy="2434320"/>
+        <a:ext cx="5356440" cy="2426040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7887,9 +8633,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>522000</xdr:colOff>
+      <xdr:colOff>513720</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7898,7 +8644,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="45360" y="51120"/>
-        <a:ext cx="6166080" cy="3468240"/>
+        <a:ext cx="6193440" cy="3459960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7917,9 +8663,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>526320</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -7928,7 +8674,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="53640" y="3595320"/>
-        <a:ext cx="6162120" cy="2685960"/>
+        <a:ext cx="6189480" cy="2677680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7942,26 +8688,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM169"/>
+  <dimension ref="A1:AM261"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4253" topLeftCell="C139" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="3449" topLeftCell="A205" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B142" activeCellId="0" sqref="B142"/>
+      <selection pane="bottomLeft" activeCell="A231" activeCellId="0" sqref="A231:A261"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="4.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="4.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="5.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="4.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="4.12"/>
@@ -7969,26 +8715,26 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="3.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="4.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="3.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="5.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="3.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="4.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="3" width="9.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="4" width="8.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="4" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="4" width="6.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="5" width="45.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="6" width="4.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="7" width="2.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="7" width="2.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="7" width="2.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="7" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="7" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="7" width="5.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="7" width="7.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="7" width="5.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="7" width="2.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="7" width="2.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="7" width="2.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="7" width="2.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="7" width="2.38"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="212.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="205.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="8"/>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -13602,237 +14348,1616 @@
         <v>221</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="112.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1" t="s">
         <v>222</v>
       </c>
       <c r="B140" s="2" t="n">
         <v>119</v>
       </c>
-      <c r="C140" s="2"/>
-      <c r="D140" s="2"/>
-      <c r="E140" s="2"/>
+      <c r="C140" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="D140" s="2" t="n">
+        <v>126</v>
+      </c>
+      <c r="E140" s="2" t="n">
+        <v>130</v>
+      </c>
       <c r="F140" s="30" t="n">
         <v>139</v>
       </c>
-      <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
-      <c r="I140" s="2"/>
-      <c r="J140" s="2"/>
-      <c r="K140" s="2"/>
-      <c r="L140" s="2"/>
-      <c r="M140" s="30" t="s">
-        <v>185</v>
+      <c r="G140" s="32" t="n">
+        <v>155</v>
+      </c>
+      <c r="H140" s="2" t="n">
+        <v>127</v>
+      </c>
+      <c r="I140" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="J140" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="K140" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="L140" s="2" t="n">
+        <v>111</v>
+      </c>
+      <c r="M140" s="30" t="n">
+        <v>125</v>
       </c>
       <c r="N140" s="2"/>
-      <c r="P140" s="2"/>
-      <c r="Q140" s="2"/>
+      <c r="O140" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="P140" s="2" t="n">
+        <v>129</v>
+      </c>
+      <c r="Q140" s="32" t="n">
+        <v>146</v>
+      </c>
       <c r="R140" s="18" t="n">
         <f aca="false">AVERAGEIF($C140:$Q140,"&gt;0")</f>
-        <v>139</v>
+        <v>129.928571428571</v>
       </c>
       <c r="U140" s="5" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="101.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C141" s="2"/>
-      <c r="D141" s="2"/>
-      <c r="E141" s="2"/>
-      <c r="F141" s="2"/>
-      <c r="G141" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="H141" s="2"/>
-      <c r="I141" s="2"/>
-      <c r="J141" s="2"/>
-      <c r="K141" s="2"/>
-      <c r="L141" s="2"/>
-      <c r="M141" s="2"/>
-      <c r="N141" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="P141" s="2"/>
-      <c r="Q141" s="2"/>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B141" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="C141" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="D141" s="32" t="n">
+        <v>165</v>
+      </c>
+      <c r="E141" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="F141" s="32" t="n">
+        <v>141</v>
+      </c>
+      <c r="G141" s="32" t="n">
+        <v>157</v>
+      </c>
+      <c r="H141" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="I141" s="2" t="n">
+        <v>128</v>
+      </c>
+      <c r="J141" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="K141" s="2" t="n">
+        <v>105</v>
+      </c>
+      <c r="L141" s="2" t="n">
+        <v>118</v>
+      </c>
+      <c r="M141" s="2" t="n">
+        <v>140</v>
+      </c>
+      <c r="N141" s="32" t="n">
+        <v>159</v>
+      </c>
+      <c r="O141" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="P141" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q141" s="32" t="n">
+        <v>160</v>
+      </c>
+      <c r="R141" s="18" t="n">
+        <f aca="false">AVERAGEIF($C141:$Q141,"&gt;0")</f>
+        <v>137.333333333333</v>
+      </c>
+      <c r="U141" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="145.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C142" s="2"/>
-      <c r="D142" s="2"/>
-      <c r="E142" s="2"/>
-      <c r="F142" s="2"/>
-      <c r="G142" s="2"/>
-      <c r="H142" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="I142" s="2"/>
-      <c r="J142" s="2"/>
-      <c r="K142" s="2"/>
-      <c r="L142" s="2"/>
-      <c r="M142" s="2"/>
-      <c r="N142" s="2"/>
-      <c r="O142" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="P142" s="2"/>
-      <c r="Q142" s="2"/>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>226</v>
+      </c>
+      <c r="B142" s="2" t="n">
+        <v>123</v>
+      </c>
+      <c r="C142" s="2" t="n">
+        <v>135</v>
+      </c>
+      <c r="D142" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="E142" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="F142" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="G142" s="2" t="n">
+        <v>134</v>
+      </c>
+      <c r="H142" s="30" t="n">
+        <v>133</v>
+      </c>
+      <c r="I142" s="32" t="n">
+        <v>142</v>
+      </c>
+      <c r="J142" s="32" t="n">
+        <v>178</v>
+      </c>
+      <c r="K142" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="L142" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="M142" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="N142" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="O142" s="32" t="n">
+        <v>154</v>
+      </c>
+      <c r="P142" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q142" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="R142" s="18" t="n">
+        <f aca="false">AVERAGEIF($C142:$Q142,"&gt;0")</f>
+        <v>134.133333333333</v>
+      </c>
+      <c r="U142" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="179.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="C143" s="2"/>
-      <c r="D143" s="2"/>
-      <c r="E143" s="2"/>
-      <c r="F143" s="2"/>
-      <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
-      <c r="I143" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="J143" s="2"/>
-      <c r="K143" s="2"/>
-      <c r="L143" s="2"/>
-      <c r="M143" s="2"/>
-      <c r="N143" s="2"/>
-      <c r="P143" s="30" t="s">
-        <v>185</v>
-      </c>
-      <c r="Q143" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="B143" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="C143" s="32" t="n">
+        <v>164</v>
+      </c>
+      <c r="D143" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="E143" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="F143" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="G143" s="2" t="n">
+        <v>137</v>
+      </c>
+      <c r="H143" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="I143" s="32" t="n">
+        <v>153</v>
+      </c>
+      <c r="J143" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="K143" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="L143" s="2" t="n">
+        <v>107</v>
+      </c>
+      <c r="M143" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="N143" s="2" t="n">
+        <v>135</v>
+      </c>
+      <c r="O143" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="P143" s="30" t="n">
+        <v>130</v>
+      </c>
+      <c r="Q143" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="R143" s="18" t="n">
+        <f aca="false">AVERAGEIF($C143:$Q143,"&gt;0")</f>
+        <v>129.4</v>
+      </c>
+      <c r="U143" s="5" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
+      </c>
+      <c r="B144" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="C144" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D144" s="2"/>
+      <c r="E144" s="2"/>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+      <c r="H144" s="2"/>
+      <c r="I144" s="2"/>
+      <c r="J144" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="K144" s="2"/>
+      <c r="L144" s="2"/>
+      <c r="M144" s="2"/>
+      <c r="N144" s="2"/>
+      <c r="P144" s="2"/>
+      <c r="Q144" s="30" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>231</v>
+      </c>
+      <c r="B145" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="C145" s="2"/>
+      <c r="D145" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E145" s="2"/>
+      <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
+      <c r="H145" s="2"/>
+      <c r="I145" s="2"/>
+      <c r="J145" s="2"/>
+      <c r="K145" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="L145" s="2"/>
+      <c r="M145" s="2"/>
+      <c r="N145" s="2"/>
+      <c r="P145" s="2"/>
+      <c r="Q145" s="2"/>
+    </row>
+    <row r="146" customFormat="false" ht="123.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
+      </c>
+      <c r="B146" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="C146" s="32" t="n">
+        <v>150</v>
+      </c>
+      <c r="D146" s="2"/>
+      <c r="E146" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2" t="n">
+        <v>131</v>
+      </c>
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2" t="n">
+        <v>122</v>
+      </c>
+      <c r="K146" s="2" t="n">
+        <v>117</v>
+      </c>
+      <c r="L146" s="30" t="n">
+        <v>120</v>
+      </c>
+      <c r="M146" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="N146" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="O146" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="P146" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="Q146" s="32" t="n">
+        <v>145</v>
+      </c>
+      <c r="R146" s="18" t="n">
+        <f aca="false">AVERAGEIF($C146:$Q146,"&gt;0")</f>
+        <v>128</v>
+      </c>
+      <c r="U146" s="5" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>234</v>
+      </c>
+      <c r="B147" s="2" t="n">
+        <v>119</v>
+      </c>
+      <c r="C147" s="2" t="n">
+        <v>132</v>
+      </c>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+      <c r="F147" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="G147" s="2"/>
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+      <c r="J147" s="2"/>
+      <c r="K147" s="2"/>
+      <c r="L147" s="2"/>
+      <c r="M147" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="N147" s="2"/>
+      <c r="P147" s="2"/>
+      <c r="Q147" s="2"/>
+      <c r="R147" s="18" t="n">
+        <f aca="false">AVERAGEIF($C147:$Q147,"&gt;0")</f>
+        <v>132</v>
+      </c>
+      <c r="U147" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="56.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1" t="s">
-        <v>231</v>
+        <v>236</v>
+      </c>
+      <c r="B148" s="2" t="n">
+        <v>108</v>
+      </c>
+      <c r="C148" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="D148" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="E148" s="2" t="n">
+        <v>130</v>
+      </c>
+      <c r="F148" s="2" t="n">
+        <v>140</v>
+      </c>
+      <c r="G148" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+      <c r="J148" s="2"/>
+      <c r="K148" s="2"/>
+      <c r="L148" s="2"/>
+      <c r="M148" s="2" t="n">
+        <v>145</v>
+      </c>
+      <c r="N148" s="30" t="n">
+        <v>137</v>
+      </c>
+      <c r="O148" s="7" t="n">
+        <v>125</v>
+      </c>
+      <c r="P148" s="2" t="n">
+        <v>115</v>
+      </c>
+      <c r="Q148" s="2" t="n">
+        <v>110</v>
+      </c>
+      <c r="R148" s="18" t="n">
+        <f aca="false">AVERAGEIF($C148:$Q148,"&gt;0")</f>
+        <v>128</v>
+      </c>
+      <c r="U148" s="5" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1" t="s">
-        <v>232</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+      <c r="E149" s="2"/>
+      <c r="F149" s="2"/>
+      <c r="G149" s="2"/>
+      <c r="H149" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I149" s="2"/>
+      <c r="J149" s="2"/>
+      <c r="K149" s="2"/>
+      <c r="L149" s="2"/>
+      <c r="M149" s="2"/>
+      <c r="N149" s="2"/>
+      <c r="O149" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P149" s="2"/>
+      <c r="Q149" s="2"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>233</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+      <c r="E150" s="2"/>
+      <c r="F150" s="2"/>
+      <c r="G150" s="2"/>
+      <c r="H150" s="2"/>
+      <c r="I150" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="J150" s="2"/>
+      <c r="K150" s="2"/>
+      <c r="L150" s="2"/>
+      <c r="M150" s="2"/>
+      <c r="N150" s="2"/>
+      <c r="P150" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q150" s="2"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1" t="s">
-        <v>234</v>
+        <v>240</v>
+      </c>
+      <c r="C151" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D151" s="2"/>
+      <c r="E151" s="2"/>
+      <c r="F151" s="2"/>
+      <c r="G151" s="2"/>
+      <c r="H151" s="2"/>
+      <c r="I151" s="2"/>
+      <c r="J151" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="K151" s="2"/>
+      <c r="L151" s="2"/>
+      <c r="M151" s="2"/>
+      <c r="N151" s="2"/>
+      <c r="P151" s="2"/>
+      <c r="Q151" s="30" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="1" t="s">
-        <v>235</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="C152" s="2"/>
+      <c r="D152" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
+      <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+      <c r="J152" s="2"/>
+      <c r="K152" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="L152" s="2"/>
+      <c r="M152" s="2"/>
+      <c r="N152" s="2"/>
+      <c r="P152" s="2"/>
+      <c r="Q152" s="2"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>236</v>
+        <v>242</v>
+      </c>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+      <c r="E153" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="F153" s="2"/>
+      <c r="G153" s="2"/>
+      <c r="H153" s="2"/>
+      <c r="I153" s="2"/>
+      <c r="J153" s="2"/>
+      <c r="K153" s="2"/>
+      <c r="L153" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="M153" s="2"/>
+      <c r="N153" s="2"/>
+      <c r="P153" s="2"/>
+      <c r="Q153" s="2"/>
+      <c r="U153" s="5" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>237</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="C154" s="2"/>
+      <c r="D154" s="2"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2"/>
+      <c r="K154" s="2"/>
+      <c r="L154" s="2"/>
+      <c r="M154" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="N154" s="2"/>
+      <c r="P154" s="2"/>
+      <c r="Q154" s="2"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>238</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="C155" s="2"/>
+      <c r="D155" s="2"/>
+      <c r="E155" s="2"/>
+      <c r="F155" s="2"/>
+      <c r="G155" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="H155" s="2"/>
+      <c r="I155" s="2"/>
+      <c r="J155" s="2"/>
+      <c r="K155" s="2"/>
+      <c r="L155" s="2"/>
+      <c r="M155" s="2"/>
+      <c r="N155" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P155" s="2"/>
+      <c r="Q155" s="2"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>239</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="C156" s="2"/>
+      <c r="D156" s="2"/>
+      <c r="E156" s="2"/>
+      <c r="F156" s="2"/>
+      <c r="G156" s="2"/>
+      <c r="H156" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I156" s="2"/>
+      <c r="J156" s="2"/>
+      <c r="K156" s="2"/>
+      <c r="L156" s="2"/>
+      <c r="M156" s="2"/>
+      <c r="N156" s="2"/>
+      <c r="O156" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P156" s="2"/>
+      <c r="Q156" s="2"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>240</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+      <c r="H157" s="2"/>
+      <c r="I157" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="J157" s="2"/>
+      <c r="K157" s="2"/>
+      <c r="L157" s="2"/>
+      <c r="M157" s="2"/>
+      <c r="N157" s="2"/>
+      <c r="P157" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q157" s="2"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>241</v>
+        <v>248</v>
+      </c>
+      <c r="B158" s="2" t="n">
+        <v>120</v>
+      </c>
+      <c r="C158" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+      <c r="H158" s="2"/>
+      <c r="I158" s="2"/>
+      <c r="J158" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="K158" s="2"/>
+      <c r="L158" s="2"/>
+      <c r="M158" s="2"/>
+      <c r="N158" s="2"/>
+      <c r="P158" s="2"/>
+      <c r="Q158" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="U158" s="5" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>242</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="B159" s="2" t="n">
+        <v>125</v>
+      </c>
+      <c r="C159" s="2"/>
+      <c r="D159" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E159" s="2"/>
+      <c r="F159" s="2"/>
+      <c r="G159" s="2"/>
+      <c r="H159" s="2"/>
+      <c r="I159" s="2"/>
+      <c r="J159" s="2"/>
+      <c r="K159" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="L159" s="2"/>
+      <c r="M159" s="2"/>
+      <c r="N159" s="2"/>
+      <c r="P159" s="2"/>
+      <c r="Q159" s="2"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>243</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2"/>
+      <c r="K160" s="2"/>
+      <c r="L160" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="M160" s="2"/>
+      <c r="N160" s="2"/>
+      <c r="P160" s="2"/>
+      <c r="Q160" s="2"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>244</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="C161" s="2"/>
+      <c r="D161" s="2"/>
+      <c r="E161" s="2"/>
+      <c r="F161" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="G161" s="2"/>
+      <c r="H161" s="2"/>
+      <c r="I161" s="2"/>
+      <c r="J161" s="2"/>
+      <c r="K161" s="2"/>
+      <c r="L161" s="2"/>
+      <c r="M161" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="N161" s="2"/>
+      <c r="P161" s="2"/>
+      <c r="Q161" s="2"/>
+      <c r="U161" s="7"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>245</v>
+        <v>253</v>
+      </c>
+      <c r="C162" s="2"/>
+      <c r="D162" s="2"/>
+      <c r="E162" s="2"/>
+      <c r="F162" s="2"/>
+      <c r="G162" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="H162" s="2"/>
+      <c r="I162" s="2"/>
+      <c r="J162" s="2"/>
+      <c r="K162" s="2"/>
+      <c r="L162" s="2"/>
+      <c r="M162" s="2"/>
+      <c r="N162" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P162" s="2"/>
+      <c r="Q162" s="2"/>
+      <c r="U162" s="5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>246</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="C163" s="2"/>
+      <c r="D163" s="2"/>
+      <c r="E163" s="2"/>
+      <c r="F163" s="2"/>
+      <c r="G163" s="2"/>
+      <c r="H163" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I163" s="2"/>
+      <c r="J163" s="2"/>
+      <c r="K163" s="2"/>
+      <c r="L163" s="2"/>
+      <c r="M163" s="2"/>
+      <c r="N163" s="2"/>
+      <c r="O163" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P163" s="2"/>
+      <c r="Q163" s="2"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>247</v>
+        <v>256</v>
+      </c>
+      <c r="C164" s="2"/>
+      <c r="D164" s="2"/>
+      <c r="E164" s="2"/>
+      <c r="F164" s="2"/>
+      <c r="G164" s="2"/>
+      <c r="H164" s="2"/>
+      <c r="I164" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="J164" s="2"/>
+      <c r="K164" s="2"/>
+      <c r="L164" s="2"/>
+      <c r="M164" s="2"/>
+      <c r="N164" s="2"/>
+      <c r="P164" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q164" s="2"/>
+      <c r="U164" s="5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>248</v>
+        <v>257</v>
+      </c>
+      <c r="C165" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D165" s="2"/>
+      <c r="E165" s="2"/>
+      <c r="F165" s="2"/>
+      <c r="G165" s="2"/>
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
+      <c r="J165" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="K165" s="2"/>
+      <c r="L165" s="2"/>
+      <c r="M165" s="2"/>
+      <c r="N165" s="2"/>
+      <c r="P165" s="2"/>
+      <c r="U165" s="5" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>249</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="C166" s="2"/>
+      <c r="D166" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E166" s="2"/>
+      <c r="F166" s="2"/>
+      <c r="G166" s="2"/>
+      <c r="H166" s="2"/>
+      <c r="I166" s="2"/>
+      <c r="J166" s="2"/>
+      <c r="K166" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="L166" s="2"/>
+      <c r="M166" s="2"/>
+      <c r="N166" s="2"/>
+      <c r="P166" s="2"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>250</v>
-      </c>
+        <v>259</v>
+      </c>
+      <c r="C167" s="2"/>
+      <c r="D167" s="2"/>
+      <c r="E167" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="F167" s="2"/>
+      <c r="G167" s="2"/>
+      <c r="H167" s="2"/>
+      <c r="I167" s="2"/>
+      <c r="J167" s="2"/>
+      <c r="K167" s="2"/>
+      <c r="L167" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="M167" s="2"/>
+      <c r="N167" s="2"/>
+      <c r="P167" s="2"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>251</v>
-      </c>
+        <v>260</v>
+      </c>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
+      <c r="F168" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="G168" s="2"/>
+      <c r="H168" s="2"/>
+      <c r="I168" s="2"/>
+      <c r="J168" s="2"/>
+      <c r="K168" s="2"/>
+      <c r="L168" s="2"/>
+      <c r="M168" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="N168" s="2"/>
+      <c r="P168" s="2"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>252</v>
+        <v>261</v>
+      </c>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="H169" s="2"/>
+      <c r="I169" s="2"/>
+      <c r="J169" s="2"/>
+      <c r="K169" s="2"/>
+      <c r="L169" s="2"/>
+      <c r="M169" s="2"/>
+      <c r="N169" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P169" s="2"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C170" s="2"/>
+      <c r="D170" s="2"/>
+      <c r="E170" s="2"/>
+      <c r="F170" s="2"/>
+      <c r="G170" s="2"/>
+      <c r="H170" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I170" s="2"/>
+      <c r="J170" s="2"/>
+      <c r="K170" s="2"/>
+      <c r="L170" s="2"/>
+      <c r="M170" s="2"/>
+      <c r="N170" s="2"/>
+      <c r="O170" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P170" s="2"/>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C171" s="2"/>
+      <c r="D171" s="2"/>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
+      <c r="G171" s="2"/>
+      <c r="H171" s="2"/>
+      <c r="I171" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="J171" s="2"/>
+      <c r="K171" s="2"/>
+      <c r="L171" s="2"/>
+      <c r="M171" s="2"/>
+      <c r="N171" s="2"/>
+      <c r="P171" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="U171" s="0"/>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C172" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="D172" s="2"/>
+      <c r="E172" s="2"/>
+      <c r="F172" s="2"/>
+      <c r="G172" s="2"/>
+      <c r="H172" s="2"/>
+      <c r="I172" s="2"/>
+      <c r="J172" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="K172" s="2"/>
+      <c r="L172" s="2"/>
+      <c r="M172" s="2"/>
+      <c r="N172" s="2"/>
+      <c r="P172" s="2"/>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C173" s="2"/>
+      <c r="D173" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E173" s="2"/>
+      <c r="F173" s="2"/>
+      <c r="G173" s="2"/>
+      <c r="H173" s="2"/>
+      <c r="I173" s="2"/>
+      <c r="J173" s="2"/>
+      <c r="K173" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="L173" s="2"/>
+      <c r="M173" s="2"/>
+      <c r="N173" s="2"/>
+      <c r="P173" s="2"/>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C174" s="2"/>
+      <c r="D174" s="2"/>
+      <c r="E174" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="F174" s="2"/>
+      <c r="G174" s="2"/>
+      <c r="H174" s="2"/>
+      <c r="I174" s="2"/>
+      <c r="J174" s="2"/>
+      <c r="K174" s="2"/>
+      <c r="L174" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="M174" s="2"/>
+      <c r="N174" s="2"/>
+      <c r="P174" s="2"/>
+      <c r="U174" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C175" s="2"/>
+      <c r="D175" s="2"/>
+      <c r="E175" s="2"/>
+      <c r="F175" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="G175" s="2"/>
+      <c r="H175" s="2"/>
+      <c r="I175" s="2"/>
+      <c r="J175" s="2"/>
+      <c r="K175" s="2"/>
+      <c r="L175" s="2"/>
+      <c r="M175" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="N175" s="2"/>
+      <c r="P175" s="2"/>
+      <c r="U175" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B176" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
+      <c r="E176" s="2"/>
+      <c r="F176" s="2"/>
+      <c r="G176" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="H176" s="2"/>
+      <c r="I176" s="2"/>
+      <c r="J176" s="2"/>
+      <c r="K176" s="2"/>
+      <c r="L176" s="2"/>
+      <c r="M176" s="2"/>
+      <c r="N176" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P176" s="2"/>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C177" s="2"/>
+      <c r="D177" s="2"/>
+      <c r="E177" s="2"/>
+      <c r="F177" s="2"/>
+      <c r="G177" s="2"/>
+      <c r="H177" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="I177" s="2"/>
+      <c r="J177" s="2"/>
+      <c r="K177" s="2"/>
+      <c r="L177" s="2"/>
+      <c r="M177" s="2"/>
+      <c r="N177" s="2"/>
+      <c r="O177" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="P177" s="2"/>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
+      <c r="E178" s="2"/>
+      <c r="F178" s="2"/>
+      <c r="G178" s="2"/>
+      <c r="H178" s="2"/>
+      <c r="I178" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="J178" s="2"/>
+      <c r="K178" s="2"/>
+      <c r="L178" s="2"/>
+      <c r="M178" s="2"/>
+      <c r="N178" s="2"/>
+      <c r="P178" s="30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="U181" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="U182" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="U187" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="U189" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="U193" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="U195" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="U196" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="U202" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="U205" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="U208" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="U209" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="U210" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A215" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="U215" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A216" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="U216" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A217" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A221" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="U221" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A222" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A223" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="U223" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A224" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A225" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A226" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="U230" s="41" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A231" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A232" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A233" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A234" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A235" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A236" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A237" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A238" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A239" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A240" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A241" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A242" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A243" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A257" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A258" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A259" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A260" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A261" s="1" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -13852,208 +15977,208 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="A231:A261 C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="5.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="8.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="4" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="7" width="9.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="197.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
+      <c r="A1" s="42"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="43" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>254</v>
+      <c r="B2" s="44" t="s">
+        <v>364</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>365</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="45" t="n">
+      <c r="A3" s="46" t="n">
         <f aca="true">TODAY()</f>
-        <v>45383</v>
-      </c>
-      <c r="B3" s="46" t="s">
+        <v>45473</v>
+      </c>
+      <c r="B3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="47" t="n">
+      <c r="C3" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!B$3:B$159, "&gt;0")</f>
-        <v>116.786324786325</v>
+        <v>116.92125984252</v>
       </c>
       <c r="D3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="47" t="n">
+      <c r="C4" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!C$3:C$153, "&gt;0")</f>
-        <v>131.114285714286</v>
+        <v>132.857142857143</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="47" t="n">
+      <c r="C5" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!D$3:D$153, "&gt;0")</f>
-        <v>136.75</v>
+        <v>136.736842105263</v>
       </c>
       <c r="D5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="47" t="n">
+      <c r="C6" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!E$3:E$153, "&gt;0")</f>
-        <v>126.384615384615</v>
+        <v>126.964912280702</v>
       </c>
       <c r="D6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="47" t="n">
+      <c r="C7" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!F$3:F$153, "&gt;0")</f>
-        <v>128.036363636364</v>
+        <v>128.64406779661</v>
       </c>
       <c r="D7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="47" t="n">
+      <c r="C8" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!G$3:G$153, "&gt;0")</f>
-        <v>118.754385964912</v>
+        <v>120.693548387097</v>
       </c>
       <c r="D8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="48" t="s">
+      <c r="B9" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="47" t="n">
+      <c r="C9" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!H$3:H$153, "&gt;0")</f>
-        <v>133.759259259259</v>
+        <v>133.672413793103</v>
       </c>
       <c r="D9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="47" t="n">
+      <c r="C10" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!I$3:I$153, "&gt;0")</f>
-        <v>126.163265306122</v>
+        <v>126.924528301887</v>
       </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="47" t="n">
+      <c r="C11" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!J$3:J$153, "&gt;0")</f>
-        <v>130.391304347826</v>
+        <v>130.372549019608</v>
       </c>
       <c r="D11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="47" t="n">
+      <c r="C12" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!K$3:K$153, "&gt;0")</f>
-        <v>125.017543859649</v>
+        <v>124.338709677419</v>
       </c>
       <c r="D12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="47" t="n">
+      <c r="C13" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!L$3:L$153, "&gt;0")</f>
-        <v>125.032786885246</v>
+        <v>124.242424242424</v>
       </c>
       <c r="D13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="47" t="n">
+      <c r="C14" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!M$3:M$153, "&gt;0")</f>
-        <v>126.096153846154</v>
+        <v>126.293103448276</v>
       </c>
       <c r="D14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="47" t="n">
+      <c r="C15" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!N$3:N$153, "&gt;0")</f>
-        <v>121.730769230769</v>
+        <v>122.859649122807</v>
       </c>
       <c r="D15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="47" t="n">
+      <c r="C16" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!O$3:O$153, "&gt;0")</f>
-        <v>125.68085106383</v>
+        <v>126.377358490566</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="47" t="n">
+      <c r="C17" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!P$3:P$153, "&gt;0")</f>
-        <v>136.5</v>
+        <v>135.102941176471</v>
       </c>
       <c r="D17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="47" t="n">
+      <c r="C18" s="48" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!Q$3:Q$159, "&gt;0")</f>
-        <v>124.734375</v>
+        <v>125.728571428571</v>
       </c>
       <c r="D18" s="7"/>
     </row>
@@ -14072,7 +16197,7 @@
         <v>10</v>
       </c>
       <c r="U95" s="7" t="s">
-        <v>255</v>
+        <v>366</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14081,7 +16206,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="79.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="U112" s="49" t="s">
+      <c r="U112" s="50" t="s">
         <v>136</v>
       </c>
     </row>
@@ -14089,8 +16214,8 @@
       <c r="P113" s="7" t="n">
         <v>117</v>
       </c>
-      <c r="U113" s="49" t="s">
-        <v>256</v>
+      <c r="U113" s="50" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14117,27 +16242,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="1" sqref="A231:A261 A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="4.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="7" width="3.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="5" style="7" width="3.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="7" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="7" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="7" width="3.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="7" width="3.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="7" width="4.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="7" width="4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="7" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="7" width="3.88"/>
   </cols>
   <sheetData>
@@ -14152,7 +16277,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>257</v>
+        <v>368</v>
       </c>
       <c r="E1" s="2" t="n">
         <v>0</v>
@@ -14199,7 +16324,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>257</v>
+        <v>368</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
@@ -14246,7 +16371,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>257</v>
+        <v>368</v>
       </c>
       <c r="G3" s="2" t="n">
         <v>0</v>
@@ -14293,7 +16418,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>257</v>
+        <v>368</v>
       </c>
       <c r="H4" s="2" t="n">
         <v>0</v>
@@ -14340,7 +16465,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>257</v>
+        <v>368</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>0</v>
@@ -14387,7 +16512,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>257</v>
+        <v>368</v>
       </c>
       <c r="J6" s="2" t="n">
         <v>0</v>
@@ -14434,7 +16559,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>257</v>
+        <v>368</v>
       </c>
       <c r="K7" s="2" t="n">
         <v>0</v>
@@ -14610,17 +16735,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
+      <selection pane="topLeft" activeCell="I37" activeCellId="1" sqref="A231:A261 I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="7" width="8.48"/>
   </cols>

</xml_diff>

<commit_message>
Add more glucose values
</commit_message>
<xml_diff>
--- a/polynomial-trendlines/all-day-glucose.xlsx
+++ b/polynomial-trendlines/all-day-glucose.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="370">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -2029,12 +2029,12 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2120,7 +2120,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2285,10 +2285,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2397,7 +2393,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2427,7 +2423,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.147726511752494"/>
+          <c:x val="0.147803375301366"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -2446,10 +2442,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.108283667046139"/>
-          <c:y val="0.188851792713021"/>
-          <c:w val="0.696243219714726"/>
-          <c:h val="0.542168674698795"/>
+          <c:x val="0.108290918832039"/>
+          <c:y val="0.188879210220674"/>
+          <c:w val="0.696222877042593"/>
+          <c:h val="0.542102206736353"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3499,11 +3495,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="13385115"/>
-        <c:axId val="20506864"/>
+        <c:axId val="54216825"/>
+        <c:axId val="84646826"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13385115"/>
+        <c:axId val="54216825"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3531,7 +3527,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20506864"/>
+        <c:crossAx val="84646826"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3539,7 +3535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20506864"/>
+        <c:axId val="84646826"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="155"/>
@@ -3580,8 +3576,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0217638786580058"/>
-              <c:y val="0.196835534910727"/>
+              <c:x val="0.0217653361907313"/>
+              <c:y val="0.1965737514518"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3614,7 +3610,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13385115"/>
+        <c:crossAx val="54216825"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -3676,7 +3672,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart69.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3706,7 +3702,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.228683757883529"/>
+          <c:x val="0.22870249017038"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -3725,10 +3721,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.118519125235482"/>
-          <c:y val="0.18919312554617"/>
-          <c:w val="0.638791055778524"/>
-          <c:h val="0.54675211185552"/>
+          <c:x val="0.118528833551769"/>
+          <c:y val="0.189220684632192"/>
+          <c:w val="0.638761467889908"/>
+          <c:h val="0.546686088856519"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -3841,9 +3837,9 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>'all-day-glucose'!$A$3:$A$170</c:f>
+              <c:f>'all-day-glucose'!$A$3:$A$263</c:f>
               <c:strCache>
-                <c:ptCount val="168"/>
+                <c:ptCount val="261"/>
                 <c:pt idx="0">
                   <c:v>2023-11-08</c:v>
                 </c:pt>
@@ -4347,16 +4343,295 @@
                 </c:pt>
                 <c:pt idx="167">
                   <c:v>2024-05-01</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>2024-05-02</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>2024-05-03</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2024-05-04</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2024-05-05</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>2024-05-06</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>2024-05-07</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>2024-05-08</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>2024-05-09</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2024-05-10</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>2024-05-11</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>2024-05-12</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2024-05-13</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>2024-05-14</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2024-05-15</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>2024-05-16</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2024-05-17</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2024-05-18</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>2024-05-19</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2024-05-20</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>2024-05-21</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>2024-05-22</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>2024-05-23</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>2024-05-24</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2024-05-25</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>2024-05-26</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2024-05-27</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>2024-05-28</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>2024-05-29</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>2024-05-30</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>2024-05-31</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>2024-06-01</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>2024-06-02</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>2024-06-03</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2024-06-04</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>2024-06-05</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>2024-06-06</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>2024-06-07</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>2024-06-08</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>2024-06-09</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>2024-06-10</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>2024-06-11</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>2024-06-12</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>2024-06-13</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>2024-06-14</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>2024-06-15</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>2024-06-16</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>2024-06-17</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>2024-06-18</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>2024-06-19</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>2024-06-20</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>2024-06-21</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>2024-06-22</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>2024-06-23</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2024-06-24</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>2024-06-25</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>2024-06-26</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>2024-06-27</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>2024-06-28</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>2024-06-29</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>2024-06-30</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>2024-07-01</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>2024-07-02</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2024-07-03</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>2024-07-04</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>2024-07-05</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>2024-07-06</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>2024-07-07</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>2024-07-08</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>2024-07-09</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>2024-07-10</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>2024-07-11</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>2024-07-12</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>2024-07-13</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>2024-07-14</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>2024-07-15</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>2024-07-16</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>2024-07-17</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>2024-07-18</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>2024-07-19</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>2024-07-20</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>2024-07-21</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>2024-07-22</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>2024-07-23</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>2024-07-24</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>2024-07-25</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>2024-07-26</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>2024-07-27</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>2024-07-28</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>2024-07-29</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>2024-07-30</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>2024-07-31</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'all-day-glucose'!$B$3:$B$170</c:f>
+              <c:f>'all-day-glucose'!$B$3:$B$263</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="168"/>
+                <c:ptCount val="261"/>
                 <c:pt idx="1">
                   <c:v>104</c:v>
                 </c:pt>
@@ -4737,6 +5012,108 @@
                 </c:pt>
                 <c:pt idx="156">
                   <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4751,11 +5128,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="60247472"/>
-        <c:axId val="40201014"/>
+        <c:axId val="14536777"/>
+        <c:axId val="63068109"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="60247472"/>
+        <c:axId val="14536777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4783,7 +5160,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40201014"/>
+        <c:crossAx val="63068109"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4791,7 +5168,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40201014"/>
+        <c:axId val="63068109"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="160"/>
@@ -4830,7 +5207,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60247472"/>
+        <c:crossAx val="14536777"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -4892,7 +5269,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart70.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4932,10 +5309,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.138911290322581"/>
-          <c:y val="0.177893175074184"/>
-          <c:w val="0.706182795698925"/>
-          <c:h val="0.537388724035608"/>
+          <c:x val="0.138922477495633"/>
+          <c:y val="0.17791957263689"/>
+          <c:w val="0.706166868198307"/>
+          <c:h val="0.537320077162784"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -5107,11 +5484,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="10052224"/>
-        <c:axId val="20397419"/>
+        <c:axId val="57302467"/>
+        <c:axId val="77813879"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="10052224"/>
+        <c:axId val="57302467"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5141,8 +5518,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.399731182795699"/>
-              <c:y val="0.891839762611276"/>
+              <c:x val="0.399704420260648"/>
+              <c:y val="0.89182371271702"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -5175,7 +5552,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20397419"/>
+        <c:crossAx val="77813879"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5183,7 +5560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="20397419"/>
+        <c:axId val="77813879"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="110"/>
@@ -5249,7 +5626,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10052224"/>
+        <c:crossAx val="57302467"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5300,7 +5677,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5330,7 +5707,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.183841906422552"/>
+          <c:x val="0.183876022984503"/>
           <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
@@ -5349,10 +5726,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0942749200813717"/>
-          <c:y val="0.13535164377861"/>
-          <c:w val="0.706713164777681"/>
-          <c:h val="0.663129421556388"/>
+          <c:x val="0.0942596784491265"/>
+          <c:y val="0.135365726771408"/>
+          <c:w val="0.706657379998839"/>
+          <c:h val="0.663094371033191"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -6221,11 +6598,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="84307264"/>
-        <c:axId val="4167600"/>
+        <c:axId val="91028050"/>
+        <c:axId val="15971340"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="84307264"/>
+        <c:axId val="91028050"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="45413"/>
@@ -6255,7 +6632,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4167600"/>
+        <c:crossAx val="15971340"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -6265,7 +6642,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="4167600"/>
+        <c:axId val="15971340"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -6304,7 +6681,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84307264"/>
+        <c:crossAx val="91028050"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -6369,7 +6746,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6398,8 +6775,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.19285797371176"/>
-          <c:y val="0.00940986691759645"/>
+          <c:x val="0.192821465907771"/>
+          <c:y val="0.00941113202473783"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -6417,10 +6794,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.104745841572642"/>
-          <c:y val="0.115338083075682"/>
-          <c:w val="0.643422123996743"/>
-          <c:h val="0.625218443339158"/>
+          <c:x val="0.10471599488907"/>
+          <c:y val="0.115353589674644"/>
+          <c:w val="0.643396445580207"/>
+          <c:h val="0.625168055929013"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -8381,11 +8758,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="57359876"/>
-        <c:axId val="18948646"/>
+        <c:axId val="81384877"/>
+        <c:axId val="34700356"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57359876"/>
+        <c:axId val="81384877"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8413,7 +8790,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18948646"/>
+        <c:crossAx val="34700356"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8421,7 +8798,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18948646"/>
+        <c:axId val="34700356"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -8460,7 +8837,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57359876"/>
+        <c:crossAx val="81384877"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -8536,9 +8913,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>263520</xdr:colOff>
+      <xdr:colOff>263160</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2563920</xdr:rowOff>
+      <xdr:rowOff>2563560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8547,7 +8924,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="92520" y="84240"/>
-        <a:ext cx="5375520" cy="2479680"/>
+        <a:ext cx="5375160" cy="2479320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8566,9 +8943,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>2725560</xdr:colOff>
+      <xdr:colOff>2725200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2563920</xdr:rowOff>
+      <xdr:rowOff>2563560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8577,7 +8954,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5566680" y="92520"/>
-        <a:ext cx="4394880" cy="2471400"/>
+        <a:ext cx="4394520" cy="2471040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8601,9 +8978,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>744480</xdr:colOff>
+      <xdr:colOff>744120</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>2478960</xdr:rowOff>
+      <xdr:rowOff>2478600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8612,7 +8989,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="42120" y="52920"/>
-        <a:ext cx="5356440" cy="2426040"/>
+        <a:ext cx="5358600" cy="2425680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8636,9 +9013,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>513720</xdr:colOff>
+      <xdr:colOff>513360</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8647,7 +9024,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="45360" y="51120"/>
-        <a:ext cx="6193440" cy="3459960"/>
+        <a:ext cx="6202080" cy="3459600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8666,9 +9043,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8677,7 +9054,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="53640" y="3595320"/>
-        <a:ext cx="6189480" cy="2677680"/>
+        <a:ext cx="6198120" cy="2677320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8698,12 +9075,12 @@
   <dimension ref="A1:AM261"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4063" topLeftCell="A216" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="4052" topLeftCell="A216" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="U234" activeCellId="0" sqref="U234"/>
+      <selection pane="bottomLeft" activeCell="U237" activeCellId="0" sqref="U237"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="4.6"/>
@@ -15885,7 +16262,7 @@
       <c r="B230" s="2" t="n">
         <v>114</v>
       </c>
-      <c r="U230" s="41" t="s">
+      <c r="U230" s="38" t="s">
         <v>332</v>
       </c>
     </row>
@@ -15920,6 +16297,9 @@
       <c r="A234" s="1" t="s">
         <v>337</v>
       </c>
+      <c r="B234" s="2" t="n">
+        <v>101</v>
+      </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
@@ -15930,10 +16310,22 @@
       <c r="A236" s="1" t="s">
         <v>339</v>
       </c>
+      <c r="B236" s="2" t="n">
+        <v>78</v>
+      </c>
+      <c r="U236" s="5" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
         <v>340</v>
+      </c>
+      <c r="B237" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="U237" s="5" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16080,10 +16472,10 @@
   <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="1" sqref="U237 C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="5.62"/>
@@ -16093,186 +16485,186 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="197.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="42"/>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>366</v>
       </c>
       <c r="D2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="46" t="n">
+      <c r="A3" s="45" t="n">
         <f aca="true">TODAY()</f>
-        <v>45476</v>
-      </c>
-      <c r="B3" s="47" t="s">
+        <v>45480</v>
+      </c>
+      <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="48" t="n">
+      <c r="C3" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!B$3:B$159, "&gt;0")</f>
         <v>116.92125984252</v>
       </c>
       <c r="D3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="48" t="n">
+      <c r="C4" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!C$3:C$153, "&gt;0")</f>
         <v>132.857142857143</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="48" t="n">
+      <c r="C5" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!D$3:D$153, "&gt;0")</f>
         <v>136.736842105263</v>
       </c>
       <c r="D5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="48" t="n">
+      <c r="C6" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!E$3:E$153, "&gt;0")</f>
         <v>126.964912280702</v>
       </c>
       <c r="D6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="48" t="n">
+      <c r="C7" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!F$3:F$153, "&gt;0")</f>
         <v>128.64406779661</v>
       </c>
       <c r="D7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="48" t="n">
+      <c r="C8" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!G$3:G$153, "&gt;0")</f>
         <v>120.693548387097</v>
       </c>
       <c r="D8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="48" t="n">
+      <c r="C9" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!H$3:H$153, "&gt;0")</f>
         <v>133.672413793103</v>
       </c>
       <c r="D9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="48" t="n">
+      <c r="C10" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!I$3:I$153, "&gt;0")</f>
         <v>126.924528301887</v>
       </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="48" t="n">
+      <c r="C11" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!J$3:J$153, "&gt;0")</f>
         <v>130.372549019608</v>
       </c>
       <c r="D11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="48" t="n">
+      <c r="C12" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!K$3:K$153, "&gt;0")</f>
         <v>124.338709677419</v>
       </c>
       <c r="D12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="48" t="n">
+      <c r="C13" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!L$3:L$153, "&gt;0")</f>
         <v>124.242424242424</v>
       </c>
       <c r="D13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="48" t="n">
+      <c r="C14" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!M$3:M$153, "&gt;0")</f>
         <v>126.293103448276</v>
       </c>
       <c r="D14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="48" t="n">
+      <c r="C15" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!N$3:N$153, "&gt;0")</f>
         <v>122.859649122807</v>
       </c>
       <c r="D15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="48" t="n">
+      <c r="C16" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!O$3:O$153, "&gt;0")</f>
         <v>126.377358490566</v>
       </c>
       <c r="D16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="48" t="n">
+      <c r="C17" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!P$3:P$153, "&gt;0")</f>
         <v>135.102941176471</v>
       </c>
       <c r="D17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="48" t="n">
+      <c r="C18" s="47" t="n">
         <f aca="false">AVERAGEIF('all-day-glucose'!Q$3:Q$159, "&gt;0")</f>
         <v>125.728571428571</v>
       </c>
@@ -16302,7 +16694,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="79.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="U112" s="50" t="s">
+      <c r="U112" s="49" t="s">
         <v>136</v>
       </c>
     </row>
@@ -16310,7 +16702,7 @@
       <c r="P113" s="7" t="n">
         <v>117</v>
       </c>
-      <c r="U113" s="50" t="s">
+      <c r="U113" s="49" t="s">
         <v>368</v>
       </c>
     </row>
@@ -16345,10 +16737,10 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="1" sqref="U237 A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="4.12"/>
@@ -16838,10 +17230,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I37" activeCellId="0" sqref="I37"/>
+      <selection pane="topLeft" activeCell="I37" activeCellId="1" sqref="U237 I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="7" width="8.48"/>
   </cols>

</xml_diff>